<commit_message>
No Contact report update
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateNoContact.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateNoContact.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TyronR\Desktop\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E260A37-7831-4645-8C77-57231EC2FC20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC603745-382F-4D83-AEB4-DC65EBE9EABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="20115" windowHeight="13860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="897">
   <si>
     <t>PL11DMM4U</t>
   </si>
@@ -2797,6 +2797,9 @@
   </si>
   <si>
     <t>NOK Surname</t>
+  </si>
+  <si>
+    <t>Lead Status</t>
   </si>
 </sst>
 </file>
@@ -2853,7 +2856,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2971,6 +2974,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3343,7 +3352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="270">
+  <cellXfs count="275">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -3629,6 +3638,309 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="12" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="12" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="12" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="10" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="14" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="14" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="8" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="16" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="19" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="19" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="19" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="19" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="14" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="14" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="14" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="14" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="16" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="16" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="16" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="16" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3653,24 +3965,6 @@
     <xf numFmtId="0" fontId="2" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3680,293 +3974,19 @@
     <xf numFmtId="0" fontId="2" fillId="20" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="12" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="12" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="10" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="16" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="16" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="16" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="12" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="8" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="14" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="14" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="14" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="14" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="10" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="16" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="16" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="19" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="19" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="19" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="19" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="14" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="14" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4317,130 +4337,130 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="43.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="48.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="36.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="43.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="48.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="36.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="20.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="19.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="20.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="20.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="17.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="28" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="43.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="50" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="52" max="54" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="56" max="58" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="59" max="62" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="63" max="66" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="43.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="50" width="17.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="52" max="54" width="15.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="19.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="56" max="58" width="15.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="59" max="62" width="10.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="63" max="66" width="13.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="67" max="70" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="71" max="74" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="74" width="16.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="13.81640625" style="5" bestFit="1" customWidth="1"/>
     <col min="76" max="76" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="78" width="19.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="80" max="81" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="21.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="19.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="78" width="19.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="80" max="81" width="20.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="21.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="85" max="85" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="13.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="6.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="91" max="91" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="102.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="18.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="102.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="99" max="99" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="102.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="24.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="18.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="14.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="102.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="106" max="106" width="17" style="5" bestFit="1" customWidth="1"/>
     <col min="107" max="107" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="108" max="108" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="9.140625" style="2"/>
-    <col min="111" max="111" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="22.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="20.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="9.1796875" style="2"/>
+    <col min="111" max="111" width="16.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="22.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="8.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="20.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="116" max="116" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="19.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="22.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="14.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="14.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="22.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="14.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="16.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="14.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="12.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="7.81640625" style="5" bestFit="1" customWidth="1"/>
     <col min="125" max="126" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="127" max="127" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="6.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="130" max="131" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="6.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="130" max="131" width="16.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="17.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="13.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="10.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="135" max="135" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="136" max="137" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="11.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="136" max="137" width="10.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="11.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="11.1796875" style="5" bestFit="1" customWidth="1"/>
     <col min="142" max="142" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="21.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="144" max="16384" width="9.140625" style="2"/>
+    <col min="143" max="143" width="21.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="144" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:143" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:143" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>657</v>
       </c>
@@ -4871,7 +4891,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="2" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1502</v>
       </c>
@@ -5103,7 +5123,7 @@
       </c>
       <c r="EM2" s="6"/>
     </row>
-    <row r="3" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1510</v>
       </c>
@@ -5347,7 +5367,7 @@
       </c>
       <c r="EM3" s="6"/>
     </row>
-    <row r="4" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>1514</v>
       </c>
@@ -5583,7 +5603,7 @@
       </c>
       <c r="EM4" s="6"/>
     </row>
-    <row r="5" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>1515</v>
       </c>
@@ -5805,7 +5825,7 @@
       </c>
       <c r="EM5" s="6"/>
     </row>
-    <row r="6" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>1521</v>
       </c>
@@ -6039,7 +6059,7 @@
       </c>
       <c r="EM6" s="6"/>
     </row>
-    <row r="7" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>1534</v>
       </c>
@@ -6281,7 +6301,7 @@
       </c>
       <c r="EM7" s="6"/>
     </row>
-    <row r="8" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>1551</v>
       </c>
@@ -6523,7 +6543,7 @@
       </c>
       <c r="EM8" s="6"/>
     </row>
-    <row r="9" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>1552</v>
       </c>
@@ -6745,7 +6765,7 @@
       </c>
       <c r="EM9" s="6"/>
     </row>
-    <row r="10" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>1562</v>
       </c>
@@ -6983,7 +7003,7 @@
       </c>
       <c r="EM10" s="6"/>
     </row>
-    <row r="11" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>1572</v>
       </c>
@@ -7221,7 +7241,7 @@
       </c>
       <c r="EM11" s="6"/>
     </row>
-    <row r="12" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>1581</v>
       </c>
@@ -7455,7 +7475,7 @@
       </c>
       <c r="EM12" s="6"/>
     </row>
-    <row r="13" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>1598</v>
       </c>
@@ -7689,7 +7709,7 @@
       </c>
       <c r="EM13" s="6"/>
     </row>
-    <row r="14" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>1611</v>
       </c>
@@ -7911,7 +7931,7 @@
       </c>
       <c r="EM14" s="6"/>
     </row>
-    <row r="15" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>1615</v>
       </c>
@@ -8133,7 +8153,7 @@
       </c>
       <c r="EM15" s="6"/>
     </row>
-    <row r="16" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>1628</v>
       </c>
@@ -8369,7 +8389,7 @@
       </c>
       <c r="EM16" s="6"/>
     </row>
-    <row r="17" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>1636</v>
       </c>
@@ -8605,7 +8625,7 @@
       </c>
       <c r="EM17" s="6"/>
     </row>
-    <row r="18" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>1641</v>
       </c>
@@ -8831,7 +8851,7 @@
       </c>
       <c r="EM18" s="6"/>
     </row>
-    <row r="19" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>1644</v>
       </c>
@@ -9055,7 +9075,7 @@
       </c>
       <c r="EM19" s="6"/>
     </row>
-    <row r="20" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>1645</v>
       </c>
@@ -9281,7 +9301,7 @@
       </c>
       <c r="EM20" s="6"/>
     </row>
-    <row r="21" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>1658</v>
       </c>
@@ -9503,7 +9523,7 @@
       </c>
       <c r="EM21" s="6"/>
     </row>
-    <row r="22" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>1660</v>
       </c>
@@ -9737,7 +9757,7 @@
       </c>
       <c r="EM22" s="6"/>
     </row>
-    <row r="23" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>1661</v>
       </c>
@@ -9981,7 +10001,7 @@
       </c>
       <c r="EM23" s="6"/>
     </row>
-    <row r="24" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>1667</v>
       </c>
@@ -10219,7 +10239,7 @@
       </c>
       <c r="EM24" s="6"/>
     </row>
-    <row r="25" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>1670</v>
       </c>
@@ -10445,7 +10465,7 @@
       </c>
       <c r="EM25" s="6"/>
     </row>
-    <row r="26" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>1674</v>
       </c>
@@ -10675,7 +10695,7 @@
       </c>
       <c r="EM26" s="6"/>
     </row>
-    <row r="27" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>1677</v>
       </c>
@@ -10895,7 +10915,7 @@
       </c>
       <c r="EM27" s="6"/>
     </row>
-    <row r="28" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>1686</v>
       </c>
@@ -11119,7 +11139,7 @@
       </c>
       <c r="EM28" s="6"/>
     </row>
-    <row r="29" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>1687</v>
       </c>
@@ -11353,7 +11373,7 @@
       </c>
       <c r="EM29" s="6"/>
     </row>
-    <row r="30" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>1694</v>
       </c>
@@ -11585,7 +11605,7 @@
       </c>
       <c r="EM30" s="6"/>
     </row>
-    <row r="31" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>1696</v>
       </c>
@@ -11819,7 +11839,7 @@
       </c>
       <c r="EM31" s="6"/>
     </row>
-    <row r="32" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>1697</v>
       </c>
@@ -12039,7 +12059,7 @@
       </c>
       <c r="EM32" s="6"/>
     </row>
-    <row r="33" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>1700</v>
       </c>
@@ -12259,7 +12279,7 @@
       </c>
       <c r="EM33" s="6"/>
     </row>
-    <row r="34" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>1701</v>
       </c>
@@ -12481,7 +12501,7 @@
       </c>
       <c r="EM34" s="6"/>
     </row>
-    <row r="35" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>1720</v>
       </c>
@@ -12715,7 +12735,7 @@
       </c>
       <c r="EM35" s="6"/>
     </row>
-    <row r="36" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>1734</v>
       </c>
@@ -12951,7 +12971,7 @@
       </c>
       <c r="EM36" s="6"/>
     </row>
-    <row r="37" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>1736</v>
       </c>
@@ -13185,7 +13205,7 @@
       </c>
       <c r="EM37" s="6"/>
     </row>
-    <row r="38" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>1740</v>
       </c>
@@ -13419,7 +13439,7 @@
       </c>
       <c r="EM38" s="6"/>
     </row>
-    <row r="39" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:143" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>1747</v>
       </c>
@@ -13653,7 +13673,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:EM1" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState ref="A2:EM118">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:EM118">
       <sortCondition ref="DP1"/>
     </sortState>
   </autoFilter>
@@ -13664,632 +13684,638 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:CG20"/>
+  <dimension ref="A1:CH20"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="BO1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CD1" sqref="CD1:CG2"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="BR1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CI13" sqref="CI13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.28515625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="146" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.26953125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="31.1796875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="11.7265625" style="146" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="34" customWidth="1"/>
     <col min="11" max="11" width="21" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.85546875" style="42" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="46" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.28515625" style="46" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.28515625" style="46" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="37.28515625" style="46" customWidth="1"/>
-    <col min="20" max="20" width="33.7109375" style="46" customWidth="1"/>
-    <col min="21" max="21" width="12.140625" style="46" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.7109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" style="34" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.81640625" style="42" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.26953125" style="46" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.26953125" style="46" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.26953125" style="46" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="37.26953125" style="46" customWidth="1"/>
+    <col min="20" max="20" width="33.7265625" style="46" customWidth="1"/>
+    <col min="21" max="21" width="12.1796875" style="46" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.7265625" style="34" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="11" style="46" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.42578125" style="46" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="67.42578125" style="46" customWidth="1"/>
-    <col min="27" max="30" width="36.85546875" style="46" customWidth="1"/>
-    <col min="31" max="31" width="8.85546875" style="46" customWidth="1"/>
-    <col min="32" max="32" width="40.5703125" style="46" customWidth="1"/>
-    <col min="33" max="33" width="16.140625" style="46" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22.140625" style="46" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.28515625" style="34" customWidth="1"/>
-    <col min="36" max="36" width="9.85546875" style="46" customWidth="1"/>
+    <col min="25" max="25" width="12.453125" style="46" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="67.453125" style="46" customWidth="1"/>
+    <col min="27" max="30" width="36.81640625" style="46" customWidth="1"/>
+    <col min="31" max="31" width="8.81640625" style="46" customWidth="1"/>
+    <col min="32" max="32" width="40.54296875" style="46" customWidth="1"/>
+    <col min="33" max="33" width="16.1796875" style="46" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22.1796875" style="46" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.26953125" style="34" customWidth="1"/>
+    <col min="36" max="36" width="9.81640625" style="46" customWidth="1"/>
     <col min="37" max="38" width="31" style="46" customWidth="1"/>
-    <col min="39" max="39" width="9.42578125" style="46" customWidth="1"/>
-    <col min="40" max="40" width="27.140625" style="46" customWidth="1"/>
-    <col min="41" max="41" width="25.5703125" style="46" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.28515625" style="34" customWidth="1"/>
-    <col min="43" max="43" width="9.42578125" style="80" customWidth="1"/>
+    <col min="39" max="39" width="9.453125" style="46" customWidth="1"/>
+    <col min="40" max="40" width="27.1796875" style="46" customWidth="1"/>
+    <col min="41" max="41" width="25.54296875" style="46" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.26953125" style="34" customWidth="1"/>
+    <col min="43" max="43" width="9.453125" style="80" customWidth="1"/>
     <col min="44" max="44" width="16" style="80" customWidth="1"/>
-    <col min="45" max="45" width="9.5703125" style="137" customWidth="1"/>
-    <col min="46" max="46" width="9.42578125" style="46" customWidth="1"/>
-    <col min="47" max="47" width="27.140625" style="46" customWidth="1"/>
-    <col min="48" max="48" width="25.5703125" style="46" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.28515625" style="7" customWidth="1"/>
-    <col min="50" max="50" width="9.42578125" style="80" customWidth="1"/>
+    <col min="45" max="45" width="9.54296875" style="137" customWidth="1"/>
+    <col min="46" max="46" width="9.453125" style="46" customWidth="1"/>
+    <col min="47" max="47" width="27.1796875" style="46" customWidth="1"/>
+    <col min="48" max="48" width="25.54296875" style="46" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.26953125" style="7" customWidth="1"/>
+    <col min="50" max="50" width="9.453125" style="80" customWidth="1"/>
     <col min="51" max="51" width="16" style="80" customWidth="1"/>
-    <col min="52" max="52" width="9.5703125" style="137" customWidth="1"/>
-    <col min="53" max="53" width="9.42578125" style="46" customWidth="1"/>
-    <col min="54" max="54" width="27.140625" style="46" customWidth="1"/>
-    <col min="55" max="55" width="25.5703125" style="46" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="10.28515625" style="34" customWidth="1"/>
-    <col min="57" max="57" width="9.42578125" style="80" customWidth="1"/>
+    <col min="52" max="52" width="9.54296875" style="137" customWidth="1"/>
+    <col min="53" max="53" width="9.453125" style="46" customWidth="1"/>
+    <col min="54" max="54" width="27.1796875" style="46" customWidth="1"/>
+    <col min="55" max="55" width="25.54296875" style="46" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="10.26953125" style="34" customWidth="1"/>
+    <col min="57" max="57" width="9.453125" style="80" customWidth="1"/>
     <col min="58" max="58" width="16" style="80" customWidth="1"/>
-    <col min="59" max="59" width="9.5703125" style="137" customWidth="1"/>
-    <col min="60" max="60" width="9.42578125" style="46" customWidth="1"/>
-    <col min="61" max="61" width="27.140625" style="46" customWidth="1"/>
-    <col min="62" max="62" width="25.5703125" style="46" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="10.28515625" style="34" customWidth="1"/>
-    <col min="64" max="64" width="9.42578125" style="80" customWidth="1"/>
+    <col min="59" max="59" width="9.54296875" style="137" customWidth="1"/>
+    <col min="60" max="60" width="9.453125" style="46" customWidth="1"/>
+    <col min="61" max="61" width="27.1796875" style="46" customWidth="1"/>
+    <col min="62" max="62" width="25.54296875" style="46" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="10.26953125" style="34" customWidth="1"/>
+    <col min="64" max="64" width="9.453125" style="80" customWidth="1"/>
     <col min="65" max="65" width="16" style="80" customWidth="1"/>
-    <col min="66" max="66" width="9.5703125" style="137" customWidth="1"/>
-    <col min="67" max="67" width="10.42578125" style="80" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="27.140625" style="80" customWidth="1"/>
-    <col min="69" max="69" width="14.140625" style="30" customWidth="1"/>
-    <col min="70" max="70" width="12.5703125" style="34" customWidth="1"/>
-    <col min="71" max="71" width="9.85546875" style="126" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="5.7109375" style="120" customWidth="1"/>
-    <col min="73" max="73" width="6.7109375" style="126" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="8.140625" style="126" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="7.85546875" style="126" customWidth="1"/>
-    <col min="76" max="76" width="16.42578125" style="126" customWidth="1"/>
-    <col min="77" max="77" width="11.85546875" style="126" customWidth="1"/>
-    <col min="78" max="78" width="10.140625" style="126" customWidth="1"/>
-    <col min="79" max="79" width="16.28515625" style="126" customWidth="1"/>
-    <col min="80" max="80" width="11.85546875" style="126" customWidth="1"/>
-    <col min="81" max="81" width="10.5703125" style="126" customWidth="1"/>
-    <col min="82" max="16384" width="9.140625" style="7"/>
+    <col min="66" max="66" width="9.54296875" style="137" customWidth="1"/>
+    <col min="67" max="67" width="10.453125" style="80" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="27.1796875" style="80" customWidth="1"/>
+    <col min="69" max="69" width="14.1796875" style="30" customWidth="1"/>
+    <col min="70" max="70" width="12.54296875" style="34" customWidth="1"/>
+    <col min="71" max="71" width="9.81640625" style="126" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="5.7265625" style="120" customWidth="1"/>
+    <col min="73" max="73" width="6.7265625" style="126" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="8.1796875" style="126" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="7.81640625" style="126" customWidth="1"/>
+    <col min="76" max="76" width="16.453125" style="126" customWidth="1"/>
+    <col min="77" max="77" width="11.81640625" style="126" customWidth="1"/>
+    <col min="78" max="78" width="10.1796875" style="126" customWidth="1"/>
+    <col min="79" max="79" width="16.26953125" style="126" customWidth="1"/>
+    <col min="80" max="80" width="11.81640625" style="126" customWidth="1"/>
+    <col min="81" max="81" width="10.54296875" style="126" customWidth="1"/>
+    <col min="82" max="16384" width="9.1796875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="250" t="s">
+    <row r="1" spans="1:86" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="241" t="s">
         <v>805</v>
       </c>
-      <c r="B1" s="251"/>
-      <c r="C1" s="251"/>
-      <c r="D1" s="251"/>
-      <c r="E1" s="251"/>
-      <c r="F1" s="251"/>
-      <c r="G1" s="251"/>
-      <c r="H1" s="251"/>
-      <c r="I1" s="251"/>
-      <c r="J1" s="251"/>
-      <c r="K1" s="252"/>
-      <c r="L1" s="256" t="s">
+      <c r="B1" s="242"/>
+      <c r="C1" s="242"/>
+      <c r="D1" s="242"/>
+      <c r="E1" s="242"/>
+      <c r="F1" s="242"/>
+      <c r="G1" s="242"/>
+      <c r="H1" s="242"/>
+      <c r="I1" s="242"/>
+      <c r="J1" s="242"/>
+      <c r="K1" s="243"/>
+      <c r="L1" s="247" t="s">
         <v>810</v>
       </c>
-      <c r="M1" s="256"/>
-      <c r="N1" s="256"/>
-      <c r="O1" s="256"/>
-      <c r="P1" s="256"/>
-      <c r="Q1" s="258" t="s">
+      <c r="M1" s="247"/>
+      <c r="N1" s="247"/>
+      <c r="O1" s="247"/>
+      <c r="P1" s="247"/>
+      <c r="Q1" s="249" t="s">
         <v>821</v>
       </c>
-      <c r="R1" s="258"/>
-      <c r="S1" s="258"/>
-      <c r="T1" s="258"/>
-      <c r="U1" s="258"/>
-      <c r="V1" s="258"/>
-      <c r="W1" s="258"/>
-      <c r="X1" s="258"/>
-      <c r="Y1" s="258"/>
-      <c r="Z1" s="258"/>
-      <c r="AA1" s="258"/>
-      <c r="AB1" s="258"/>
-      <c r="AC1" s="258"/>
-      <c r="AD1" s="258"/>
-      <c r="AE1" s="258"/>
-      <c r="AF1" s="258"/>
-      <c r="AG1" s="258"/>
-      <c r="AH1" s="258"/>
-      <c r="AI1" s="260" t="s">
+      <c r="R1" s="249"/>
+      <c r="S1" s="249"/>
+      <c r="T1" s="249"/>
+      <c r="U1" s="249"/>
+      <c r="V1" s="249"/>
+      <c r="W1" s="249"/>
+      <c r="X1" s="249"/>
+      <c r="Y1" s="249"/>
+      <c r="Z1" s="249"/>
+      <c r="AA1" s="249"/>
+      <c r="AB1" s="249"/>
+      <c r="AC1" s="249"/>
+      <c r="AD1" s="249"/>
+      <c r="AE1" s="249"/>
+      <c r="AF1" s="249"/>
+      <c r="AG1" s="249"/>
+      <c r="AH1" s="249"/>
+      <c r="AI1" s="215" t="s">
         <v>822</v>
       </c>
-      <c r="AJ1" s="260"/>
-      <c r="AK1" s="260"/>
-      <c r="AL1" s="260"/>
-      <c r="AM1" s="262" t="s">
+      <c r="AJ1" s="215"/>
+      <c r="AK1" s="215"/>
+      <c r="AL1" s="215"/>
+      <c r="AM1" s="217" t="s">
         <v>816</v>
       </c>
-      <c r="AN1" s="262"/>
-      <c r="AO1" s="262"/>
-      <c r="AP1" s="262"/>
-      <c r="AQ1" s="262"/>
-      <c r="AR1" s="262"/>
-      <c r="AS1" s="262"/>
-      <c r="AT1" s="264" t="s">
+      <c r="AN1" s="217"/>
+      <c r="AO1" s="217"/>
+      <c r="AP1" s="217"/>
+      <c r="AQ1" s="217"/>
+      <c r="AR1" s="217"/>
+      <c r="AS1" s="217"/>
+      <c r="AT1" s="157" t="s">
         <v>817</v>
       </c>
-      <c r="AU1" s="264"/>
-      <c r="AV1" s="264"/>
-      <c r="AW1" s="264"/>
-      <c r="AX1" s="264"/>
-      <c r="AY1" s="264"/>
-      <c r="AZ1" s="264"/>
-      <c r="BA1" s="266" t="s">
+      <c r="AU1" s="157"/>
+      <c r="AV1" s="157"/>
+      <c r="AW1" s="157"/>
+      <c r="AX1" s="157"/>
+      <c r="AY1" s="157"/>
+      <c r="AZ1" s="157"/>
+      <c r="BA1" s="219" t="s">
         <v>818</v>
       </c>
-      <c r="BB1" s="266"/>
-      <c r="BC1" s="266"/>
-      <c r="BD1" s="266"/>
-      <c r="BE1" s="266"/>
-      <c r="BF1" s="266"/>
-      <c r="BG1" s="266"/>
-      <c r="BH1" s="268" t="s">
+      <c r="BB1" s="219"/>
+      <c r="BC1" s="219"/>
+      <c r="BD1" s="219"/>
+      <c r="BE1" s="219"/>
+      <c r="BF1" s="219"/>
+      <c r="BG1" s="219"/>
+      <c r="BH1" s="221" t="s">
         <v>819</v>
       </c>
-      <c r="BI1" s="268"/>
-      <c r="BJ1" s="268"/>
-      <c r="BK1" s="268"/>
-      <c r="BL1" s="268"/>
-      <c r="BM1" s="268"/>
-      <c r="BN1" s="268"/>
-      <c r="BO1" s="169" t="s">
+      <c r="BI1" s="221"/>
+      <c r="BJ1" s="221"/>
+      <c r="BK1" s="221"/>
+      <c r="BL1" s="221"/>
+      <c r="BM1" s="221"/>
+      <c r="BN1" s="221"/>
+      <c r="BO1" s="253" t="s">
         <v>825</v>
       </c>
-      <c r="BP1" s="169"/>
-      <c r="BQ1" s="169"/>
-      <c r="BR1" s="169"/>
-      <c r="BS1" s="169"/>
-      <c r="BT1" s="169"/>
-      <c r="BU1" s="169"/>
-      <c r="BV1" s="169"/>
-      <c r="BW1" s="169"/>
-      <c r="BX1" s="169"/>
-      <c r="BY1" s="169"/>
-      <c r="BZ1" s="169"/>
-      <c r="CA1" s="169"/>
-      <c r="CB1" s="169"/>
-      <c r="CC1" s="169"/>
-      <c r="CD1" s="159" t="s">
+      <c r="BP1" s="253"/>
+      <c r="BQ1" s="253"/>
+      <c r="BR1" s="253"/>
+      <c r="BS1" s="253"/>
+      <c r="BT1" s="253"/>
+      <c r="BU1" s="253"/>
+      <c r="BV1" s="253"/>
+      <c r="BW1" s="253"/>
+      <c r="BX1" s="253"/>
+      <c r="BY1" s="253"/>
+      <c r="BZ1" s="253"/>
+      <c r="CA1" s="253"/>
+      <c r="CB1" s="253"/>
+      <c r="CC1" s="253"/>
+      <c r="CD1" s="260" t="s">
         <v>891</v>
       </c>
-      <c r="CE1" s="160"/>
-      <c r="CF1" s="160"/>
-      <c r="CG1" s="161"/>
+      <c r="CE1" s="261"/>
+      <c r="CF1" s="261"/>
+      <c r="CG1" s="262"/>
+      <c r="CH1" s="270"/>
     </row>
-    <row r="2" spans="1:85" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="253"/>
-      <c r="B2" s="254"/>
-      <c r="C2" s="254"/>
-      <c r="D2" s="254"/>
-      <c r="E2" s="254"/>
-      <c r="F2" s="254"/>
-      <c r="G2" s="254"/>
-      <c r="H2" s="254"/>
-      <c r="I2" s="254"/>
-      <c r="J2" s="254"/>
-      <c r="K2" s="255"/>
-      <c r="L2" s="257"/>
-      <c r="M2" s="257"/>
-      <c r="N2" s="257"/>
-      <c r="O2" s="257"/>
-      <c r="P2" s="257"/>
-      <c r="Q2" s="259"/>
-      <c r="R2" s="259"/>
-      <c r="S2" s="259"/>
-      <c r="T2" s="259"/>
-      <c r="U2" s="259"/>
-      <c r="V2" s="259"/>
-      <c r="W2" s="259"/>
-      <c r="X2" s="259"/>
-      <c r="Y2" s="259"/>
-      <c r="Z2" s="259"/>
-      <c r="AA2" s="259"/>
-      <c r="AB2" s="259"/>
-      <c r="AC2" s="259"/>
-      <c r="AD2" s="259"/>
-      <c r="AE2" s="259"/>
-      <c r="AF2" s="259"/>
-      <c r="AG2" s="259"/>
-      <c r="AH2" s="259"/>
-      <c r="AI2" s="261"/>
-      <c r="AJ2" s="261"/>
-      <c r="AK2" s="261"/>
-      <c r="AL2" s="261"/>
-      <c r="AM2" s="263"/>
-      <c r="AN2" s="263"/>
-      <c r="AO2" s="263"/>
-      <c r="AP2" s="263"/>
-      <c r="AQ2" s="263"/>
-      <c r="AR2" s="263"/>
-      <c r="AS2" s="263"/>
-      <c r="AT2" s="265"/>
-      <c r="AU2" s="265"/>
-      <c r="AV2" s="265"/>
-      <c r="AW2" s="265"/>
-      <c r="AX2" s="265"/>
-      <c r="AY2" s="265"/>
-      <c r="AZ2" s="265"/>
-      <c r="BA2" s="267"/>
-      <c r="BB2" s="267"/>
-      <c r="BC2" s="267"/>
-      <c r="BD2" s="267"/>
-      <c r="BE2" s="267"/>
-      <c r="BF2" s="267"/>
-      <c r="BG2" s="267"/>
-      <c r="BH2" s="269"/>
-      <c r="BI2" s="269"/>
-      <c r="BJ2" s="269"/>
-      <c r="BK2" s="269"/>
-      <c r="BL2" s="269"/>
-      <c r="BM2" s="269"/>
-      <c r="BN2" s="269"/>
-      <c r="BO2" s="170"/>
-      <c r="BP2" s="170"/>
-      <c r="BQ2" s="170"/>
-      <c r="BR2" s="170"/>
-      <c r="BS2" s="170"/>
-      <c r="BT2" s="170"/>
-      <c r="BU2" s="170"/>
-      <c r="BV2" s="170"/>
-      <c r="BW2" s="170"/>
-      <c r="BX2" s="170"/>
-      <c r="BY2" s="170"/>
-      <c r="BZ2" s="170"/>
-      <c r="CA2" s="170"/>
-      <c r="CB2" s="170"/>
-      <c r="CC2" s="170"/>
-      <c r="CD2" s="162"/>
-      <c r="CE2" s="163"/>
-      <c r="CF2" s="163"/>
-      <c r="CG2" s="164"/>
+    <row r="2" spans="1:86" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="244"/>
+      <c r="B2" s="245"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="246"/>
+      <c r="L2" s="248"/>
+      <c r="M2" s="248"/>
+      <c r="N2" s="248"/>
+      <c r="O2" s="248"/>
+      <c r="P2" s="248"/>
+      <c r="Q2" s="250"/>
+      <c r="R2" s="250"/>
+      <c r="S2" s="250"/>
+      <c r="T2" s="250"/>
+      <c r="U2" s="250"/>
+      <c r="V2" s="250"/>
+      <c r="W2" s="250"/>
+      <c r="X2" s="250"/>
+      <c r="Y2" s="250"/>
+      <c r="Z2" s="250"/>
+      <c r="AA2" s="250"/>
+      <c r="AB2" s="250"/>
+      <c r="AC2" s="250"/>
+      <c r="AD2" s="250"/>
+      <c r="AE2" s="250"/>
+      <c r="AF2" s="250"/>
+      <c r="AG2" s="250"/>
+      <c r="AH2" s="250"/>
+      <c r="AI2" s="216"/>
+      <c r="AJ2" s="216"/>
+      <c r="AK2" s="216"/>
+      <c r="AL2" s="216"/>
+      <c r="AM2" s="218"/>
+      <c r="AN2" s="218"/>
+      <c r="AO2" s="218"/>
+      <c r="AP2" s="218"/>
+      <c r="AQ2" s="218"/>
+      <c r="AR2" s="218"/>
+      <c r="AS2" s="218"/>
+      <c r="AT2" s="158"/>
+      <c r="AU2" s="158"/>
+      <c r="AV2" s="158"/>
+      <c r="AW2" s="158"/>
+      <c r="AX2" s="158"/>
+      <c r="AY2" s="158"/>
+      <c r="AZ2" s="158"/>
+      <c r="BA2" s="220"/>
+      <c r="BB2" s="220"/>
+      <c r="BC2" s="220"/>
+      <c r="BD2" s="220"/>
+      <c r="BE2" s="220"/>
+      <c r="BF2" s="220"/>
+      <c r="BG2" s="220"/>
+      <c r="BH2" s="222"/>
+      <c r="BI2" s="222"/>
+      <c r="BJ2" s="222"/>
+      <c r="BK2" s="222"/>
+      <c r="BL2" s="222"/>
+      <c r="BM2" s="222"/>
+      <c r="BN2" s="222"/>
+      <c r="BO2" s="254"/>
+      <c r="BP2" s="254"/>
+      <c r="BQ2" s="254"/>
+      <c r="BR2" s="254"/>
+      <c r="BS2" s="254"/>
+      <c r="BT2" s="254"/>
+      <c r="BU2" s="254"/>
+      <c r="BV2" s="254"/>
+      <c r="BW2" s="254"/>
+      <c r="BX2" s="254"/>
+      <c r="BY2" s="254"/>
+      <c r="BZ2" s="254"/>
+      <c r="CA2" s="254"/>
+      <c r="CB2" s="254"/>
+      <c r="CC2" s="254"/>
+      <c r="CD2" s="263"/>
+      <c r="CE2" s="264"/>
+      <c r="CF2" s="264"/>
+      <c r="CG2" s="265"/>
+      <c r="CH2" s="270"/>
     </row>
-    <row r="3" spans="1:85" s="29" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="226" t="s">
+    <row r="3" spans="1:86" s="29" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="223" t="s">
         <v>808</v>
       </c>
-      <c r="B3" s="228" t="s">
+      <c r="B3" s="225" t="s">
         <v>809</v>
       </c>
-      <c r="C3" s="228" t="s">
+      <c r="C3" s="225" t="s">
         <v>801</v>
       </c>
-      <c r="D3" s="228" t="s">
+      <c r="D3" s="225" t="s">
         <v>800</v>
       </c>
-      <c r="E3" s="228" t="s">
+      <c r="E3" s="225" t="s">
         <v>807</v>
       </c>
-      <c r="F3" s="228" t="s">
+      <c r="F3" s="225" t="s">
         <v>804</v>
       </c>
-      <c r="G3" s="228" t="s">
+      <c r="G3" s="225" t="s">
         <v>826</v>
       </c>
-      <c r="H3" s="228" t="s">
+      <c r="H3" s="225" t="s">
         <v>803</v>
       </c>
-      <c r="I3" s="240" t="s">
+      <c r="I3" s="227" t="s">
         <v>802</v>
       </c>
-      <c r="J3" s="228" t="s">
+      <c r="J3" s="225" t="s">
         <v>827</v>
       </c>
-      <c r="K3" s="234" t="s">
+      <c r="K3" s="229" t="s">
         <v>820</v>
       </c>
-      <c r="L3" s="236" t="s">
+      <c r="L3" s="231" t="s">
         <v>811</v>
       </c>
-      <c r="M3" s="214" t="s">
+      <c r="M3" s="175" t="s">
         <v>812</v>
       </c>
-      <c r="N3" s="214" t="s">
+      <c r="N3" s="175" t="s">
         <v>813</v>
       </c>
-      <c r="O3" s="238" t="s">
+      <c r="O3" s="233" t="s">
         <v>814</v>
       </c>
-      <c r="P3" s="230" t="s">
+      <c r="P3" s="235" t="s">
         <v>815</v>
       </c>
-      <c r="Q3" s="232" t="s">
+      <c r="Q3" s="237" t="s">
         <v>669</v>
       </c>
-      <c r="R3" s="193" t="s">
+      <c r="R3" s="239" t="s">
         <v>670</v>
       </c>
-      <c r="S3" s="193" t="s">
+      <c r="S3" s="239" t="s">
         <v>824</v>
       </c>
-      <c r="T3" s="193" t="s">
+      <c r="T3" s="239" t="s">
         <v>828</v>
       </c>
-      <c r="U3" s="193" t="s">
+      <c r="U3" s="239" t="s">
         <v>866</v>
       </c>
-      <c r="V3" s="242" t="s">
+      <c r="V3" s="251" t="s">
         <v>823</v>
       </c>
-      <c r="W3" s="193" t="s">
+      <c r="W3" s="239" t="s">
         <v>867</v>
       </c>
-      <c r="X3" s="193" t="s">
+      <c r="X3" s="239" t="s">
         <v>868</v>
       </c>
-      <c r="Y3" s="193" t="s">
+      <c r="Y3" s="239" t="s">
         <v>869</v>
       </c>
-      <c r="Z3" s="193" t="s">
+      <c r="Z3" s="239" t="s">
         <v>806</v>
       </c>
-      <c r="AA3" s="193" t="s">
+      <c r="AA3" s="239" t="s">
         <v>870</v>
       </c>
-      <c r="AB3" s="193" t="s">
+      <c r="AB3" s="239" t="s">
         <v>871</v>
       </c>
-      <c r="AC3" s="193" t="s">
+      <c r="AC3" s="239" t="s">
         <v>872</v>
       </c>
-      <c r="AD3" s="193" t="s">
+      <c r="AD3" s="239" t="s">
         <v>873</v>
       </c>
-      <c r="AE3" s="193" t="s">
+      <c r="AE3" s="239" t="s">
         <v>874</v>
       </c>
-      <c r="AF3" s="193" t="s">
+      <c r="AF3" s="239" t="s">
         <v>677</v>
       </c>
-      <c r="AG3" s="193" t="s">
+      <c r="AG3" s="239" t="s">
         <v>875</v>
       </c>
-      <c r="AH3" s="195" t="s">
+      <c r="AH3" s="201" t="s">
         <v>876</v>
       </c>
-      <c r="AI3" s="197" t="s">
+      <c r="AI3" s="203" t="s">
         <v>877</v>
       </c>
-      <c r="AJ3" s="244" t="s">
+      <c r="AJ3" s="205" t="s">
         <v>878</v>
       </c>
-      <c r="AK3" s="244" t="s">
+      <c r="AK3" s="205" t="s">
         <v>879</v>
       </c>
-      <c r="AL3" s="246" t="s">
+      <c r="AL3" s="207" t="s">
         <v>880</v>
       </c>
-      <c r="AM3" s="248" t="s">
+      <c r="AM3" s="209" t="s">
         <v>829</v>
       </c>
-      <c r="AN3" s="207" t="s">
+      <c r="AN3" s="211" t="s">
         <v>830</v>
       </c>
-      <c r="AO3" s="207" t="s">
+      <c r="AO3" s="211" t="s">
         <v>831</v>
       </c>
-      <c r="AP3" s="209" t="s">
+      <c r="AP3" s="213" t="s">
         <v>881</v>
       </c>
-      <c r="AQ3" s="210" t="s">
+      <c r="AQ3" s="179" t="s">
         <v>832</v>
       </c>
-      <c r="AR3" s="210" t="s">
+      <c r="AR3" s="179" t="s">
         <v>833</v>
       </c>
-      <c r="AS3" s="212" t="s">
+      <c r="AS3" s="181" t="s">
         <v>834</v>
       </c>
-      <c r="AT3" s="199" t="s">
+      <c r="AT3" s="159" t="s">
         <v>835</v>
       </c>
-      <c r="AU3" s="201" t="s">
+      <c r="AU3" s="161" t="s">
         <v>836</v>
       </c>
-      <c r="AV3" s="201" t="s">
+      <c r="AV3" s="161" t="s">
         <v>837</v>
       </c>
-      <c r="AW3" s="205" t="s">
+      <c r="AW3" s="163" t="s">
         <v>888</v>
       </c>
-      <c r="AX3" s="185" t="s">
+      <c r="AX3" s="165" t="s">
         <v>838</v>
       </c>
-      <c r="AY3" s="185" t="s">
+      <c r="AY3" s="165" t="s">
         <v>839</v>
       </c>
-      <c r="AZ3" s="187" t="s">
+      <c r="AZ3" s="167" t="s">
         <v>840</v>
       </c>
-      <c r="BA3" s="189" t="s">
+      <c r="BA3" s="171" t="s">
         <v>841</v>
       </c>
-      <c r="BB3" s="191" t="s">
+      <c r="BB3" s="177" t="s">
         <v>842</v>
       </c>
-      <c r="BC3" s="191" t="s">
+      <c r="BC3" s="177" t="s">
         <v>843</v>
       </c>
-      <c r="BD3" s="214" t="s">
+      <c r="BD3" s="175" t="s">
         <v>889</v>
       </c>
-      <c r="BE3" s="216" t="s">
+      <c r="BE3" s="173" t="s">
         <v>844</v>
       </c>
-      <c r="BF3" s="216" t="s">
+      <c r="BF3" s="173" t="s">
         <v>845</v>
       </c>
-      <c r="BG3" s="224" t="s">
+      <c r="BG3" s="169" t="s">
         <v>846</v>
       </c>
-      <c r="BH3" s="183" t="s">
+      <c r="BH3" s="255" t="s">
         <v>847</v>
       </c>
-      <c r="BI3" s="218" t="s">
+      <c r="BI3" s="199" t="s">
         <v>848</v>
       </c>
-      <c r="BJ3" s="218" t="s">
+      <c r="BJ3" s="199" t="s">
         <v>849</v>
       </c>
-      <c r="BK3" s="220" t="s">
+      <c r="BK3" s="197" t="s">
         <v>890</v>
       </c>
-      <c r="BL3" s="222" t="s">
+      <c r="BL3" s="193" t="s">
         <v>850</v>
       </c>
-      <c r="BM3" s="222" t="s">
+      <c r="BM3" s="193" t="s">
         <v>851</v>
       </c>
-      <c r="BN3" s="203" t="s">
+      <c r="BN3" s="195" t="s">
         <v>852</v>
       </c>
-      <c r="BO3" s="177" t="s">
+      <c r="BO3" s="191" t="s">
         <v>853</v>
       </c>
-      <c r="BP3" s="179" t="s">
+      <c r="BP3" s="187" t="s">
         <v>854</v>
       </c>
-      <c r="BQ3" s="181" t="s">
+      <c r="BQ3" s="189" t="s">
         <v>855</v>
       </c>
-      <c r="BR3" s="181" t="s">
+      <c r="BR3" s="189" t="s">
         <v>856</v>
       </c>
-      <c r="BS3" s="167" t="s">
+      <c r="BS3" s="185" t="s">
         <v>857</v>
       </c>
-      <c r="BT3" s="179" t="s">
+      <c r="BT3" s="187" t="s">
         <v>858</v>
       </c>
-      <c r="BU3" s="167" t="s">
+      <c r="BU3" s="185" t="s">
         <v>755</v>
       </c>
-      <c r="BV3" s="167" t="s">
+      <c r="BV3" s="185" t="s">
         <v>766</v>
       </c>
-      <c r="BW3" s="167" t="s">
+      <c r="BW3" s="185" t="s">
         <v>859</v>
       </c>
-      <c r="BX3" s="167" t="s">
+      <c r="BX3" s="185" t="s">
         <v>860</v>
       </c>
-      <c r="BY3" s="167" t="s">
+      <c r="BY3" s="185" t="s">
         <v>861</v>
       </c>
-      <c r="BZ3" s="167" t="s">
+      <c r="BZ3" s="185" t="s">
         <v>862</v>
       </c>
-      <c r="CA3" s="167" t="s">
+      <c r="CA3" s="185" t="s">
         <v>863</v>
       </c>
-      <c r="CB3" s="167" t="s">
+      <c r="CB3" s="185" t="s">
         <v>864</v>
       </c>
-      <c r="CC3" s="165" t="s">
+      <c r="CC3" s="183" t="s">
         <v>865</v>
       </c>
-      <c r="CD3" s="174" t="s">
+      <c r="CD3" s="214" t="s">
         <v>892</v>
       </c>
-      <c r="CE3" s="174" t="s">
+      <c r="CE3" s="214" t="s">
         <v>895</v>
       </c>
-      <c r="CF3" s="174" t="s">
+      <c r="CF3" s="214" t="s">
         <v>893</v>
       </c>
-      <c r="CG3" s="157" t="s">
+      <c r="CG3" s="258" t="s">
         <v>894</v>
       </c>
+      <c r="CH3" s="271" t="s">
+        <v>896</v>
+      </c>
     </row>
-    <row r="4" spans="1:85" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="227"/>
-      <c r="B4" s="229"/>
-      <c r="C4" s="229"/>
-      <c r="D4" s="229"/>
-      <c r="E4" s="229"/>
-      <c r="F4" s="229"/>
-      <c r="G4" s="229"/>
-      <c r="H4" s="229"/>
-      <c r="I4" s="241"/>
-      <c r="J4" s="229"/>
-      <c r="K4" s="235"/>
-      <c r="L4" s="237"/>
-      <c r="M4" s="215"/>
-      <c r="N4" s="215"/>
-      <c r="O4" s="239"/>
-      <c r="P4" s="231"/>
-      <c r="Q4" s="233"/>
-      <c r="R4" s="194"/>
-      <c r="S4" s="194"/>
-      <c r="T4" s="194"/>
-      <c r="U4" s="194"/>
-      <c r="V4" s="243"/>
-      <c r="W4" s="194"/>
-      <c r="X4" s="194"/>
-      <c r="Y4" s="194"/>
-      <c r="Z4" s="194"/>
-      <c r="AA4" s="194"/>
-      <c r="AB4" s="194"/>
-      <c r="AC4" s="194"/>
-      <c r="AD4" s="194"/>
-      <c r="AE4" s="194"/>
-      <c r="AF4" s="194"/>
-      <c r="AG4" s="194"/>
-      <c r="AH4" s="196"/>
-      <c r="AI4" s="198"/>
-      <c r="AJ4" s="245"/>
-      <c r="AK4" s="245"/>
-      <c r="AL4" s="247"/>
-      <c r="AM4" s="249"/>
-      <c r="AN4" s="208"/>
-      <c r="AO4" s="208"/>
-      <c r="AP4" s="174"/>
-      <c r="AQ4" s="211"/>
-      <c r="AR4" s="211"/>
-      <c r="AS4" s="213"/>
-      <c r="AT4" s="200"/>
-      <c r="AU4" s="202"/>
-      <c r="AV4" s="202"/>
-      <c r="AW4" s="206"/>
-      <c r="AX4" s="186"/>
-      <c r="AY4" s="186"/>
-      <c r="AZ4" s="188"/>
-      <c r="BA4" s="190"/>
-      <c r="BB4" s="192"/>
-      <c r="BC4" s="192"/>
-      <c r="BD4" s="215"/>
-      <c r="BE4" s="217"/>
-      <c r="BF4" s="217"/>
-      <c r="BG4" s="225"/>
-      <c r="BH4" s="184"/>
-      <c r="BI4" s="219"/>
-      <c r="BJ4" s="219"/>
-      <c r="BK4" s="221"/>
-      <c r="BL4" s="223"/>
-      <c r="BM4" s="223"/>
-      <c r="BN4" s="204"/>
-      <c r="BO4" s="178"/>
-      <c r="BP4" s="180"/>
-      <c r="BQ4" s="182"/>
-      <c r="BR4" s="182"/>
-      <c r="BS4" s="168"/>
-      <c r="BT4" s="180"/>
-      <c r="BU4" s="168"/>
-      <c r="BV4" s="168"/>
-      <c r="BW4" s="168"/>
-      <c r="BX4" s="168"/>
-      <c r="BY4" s="168"/>
-      <c r="BZ4" s="168"/>
-      <c r="CA4" s="168"/>
-      <c r="CB4" s="168"/>
-      <c r="CC4" s="166"/>
-      <c r="CD4" s="175"/>
-      <c r="CE4" s="175"/>
-      <c r="CF4" s="175"/>
-      <c r="CG4" s="158"/>
+    <row r="4" spans="1:86" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="224"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="228"/>
+      <c r="J4" s="226"/>
+      <c r="K4" s="230"/>
+      <c r="L4" s="232"/>
+      <c r="M4" s="176"/>
+      <c r="N4" s="176"/>
+      <c r="O4" s="234"/>
+      <c r="P4" s="236"/>
+      <c r="Q4" s="238"/>
+      <c r="R4" s="240"/>
+      <c r="S4" s="240"/>
+      <c r="T4" s="240"/>
+      <c r="U4" s="240"/>
+      <c r="V4" s="252"/>
+      <c r="W4" s="240"/>
+      <c r="X4" s="240"/>
+      <c r="Y4" s="240"/>
+      <c r="Z4" s="240"/>
+      <c r="AA4" s="240"/>
+      <c r="AB4" s="240"/>
+      <c r="AC4" s="240"/>
+      <c r="AD4" s="240"/>
+      <c r="AE4" s="240"/>
+      <c r="AF4" s="240"/>
+      <c r="AG4" s="240"/>
+      <c r="AH4" s="202"/>
+      <c r="AI4" s="204"/>
+      <c r="AJ4" s="206"/>
+      <c r="AK4" s="206"/>
+      <c r="AL4" s="208"/>
+      <c r="AM4" s="210"/>
+      <c r="AN4" s="212"/>
+      <c r="AO4" s="212"/>
+      <c r="AP4" s="214"/>
+      <c r="AQ4" s="180"/>
+      <c r="AR4" s="180"/>
+      <c r="AS4" s="182"/>
+      <c r="AT4" s="160"/>
+      <c r="AU4" s="162"/>
+      <c r="AV4" s="162"/>
+      <c r="AW4" s="164"/>
+      <c r="AX4" s="166"/>
+      <c r="AY4" s="166"/>
+      <c r="AZ4" s="168"/>
+      <c r="BA4" s="172"/>
+      <c r="BB4" s="178"/>
+      <c r="BC4" s="178"/>
+      <c r="BD4" s="176"/>
+      <c r="BE4" s="174"/>
+      <c r="BF4" s="174"/>
+      <c r="BG4" s="170"/>
+      <c r="BH4" s="256"/>
+      <c r="BI4" s="200"/>
+      <c r="BJ4" s="200"/>
+      <c r="BK4" s="198"/>
+      <c r="BL4" s="194"/>
+      <c r="BM4" s="194"/>
+      <c r="BN4" s="196"/>
+      <c r="BO4" s="192"/>
+      <c r="BP4" s="188"/>
+      <c r="BQ4" s="190"/>
+      <c r="BR4" s="190"/>
+      <c r="BS4" s="186"/>
+      <c r="BT4" s="188"/>
+      <c r="BU4" s="186"/>
+      <c r="BV4" s="186"/>
+      <c r="BW4" s="186"/>
+      <c r="BX4" s="186"/>
+      <c r="BY4" s="186"/>
+      <c r="BZ4" s="186"/>
+      <c r="CA4" s="186"/>
+      <c r="CB4" s="186"/>
+      <c r="CC4" s="184"/>
+      <c r="CD4" s="257"/>
+      <c r="CE4" s="257"/>
+      <c r="CF4" s="257"/>
+      <c r="CG4" s="259"/>
+      <c r="CH4" s="272"/>
     </row>
-    <row r="5" spans="1:85" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:86" ht="11" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22"/>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
@@ -14379,547 +14405,554 @@
       <c r="CE5" s="74"/>
       <c r="CF5" s="74"/>
       <c r="CG5" s="153"/>
+      <c r="CH5" s="273"/>
     </row>
-    <row r="6" spans="1:85" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:85" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="250" t="s">
+    <row r="6" spans="1:86" ht="11" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:86" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="241" t="s">
         <v>805</v>
       </c>
-      <c r="B7" s="251"/>
-      <c r="C7" s="251"/>
-      <c r="D7" s="251"/>
-      <c r="E7" s="251"/>
-      <c r="F7" s="251"/>
-      <c r="G7" s="251"/>
-      <c r="H7" s="251"/>
-      <c r="I7" s="251"/>
-      <c r="J7" s="251"/>
-      <c r="K7" s="252"/>
-      <c r="L7" s="256" t="s">
+      <c r="B7" s="242"/>
+      <c r="C7" s="242"/>
+      <c r="D7" s="242"/>
+      <c r="E7" s="242"/>
+      <c r="F7" s="242"/>
+      <c r="G7" s="242"/>
+      <c r="H7" s="242"/>
+      <c r="I7" s="242"/>
+      <c r="J7" s="242"/>
+      <c r="K7" s="243"/>
+      <c r="L7" s="247" t="s">
         <v>810</v>
       </c>
-      <c r="M7" s="256"/>
-      <c r="N7" s="256"/>
-      <c r="O7" s="256"/>
-      <c r="P7" s="256"/>
-      <c r="Q7" s="258" t="s">
+      <c r="M7" s="247"/>
+      <c r="N7" s="247"/>
+      <c r="O7" s="247"/>
+      <c r="P7" s="247"/>
+      <c r="Q7" s="249" t="s">
         <v>821</v>
       </c>
-      <c r="R7" s="258"/>
-      <c r="S7" s="258"/>
-      <c r="T7" s="258"/>
-      <c r="U7" s="258"/>
-      <c r="V7" s="258"/>
-      <c r="W7" s="258"/>
-      <c r="X7" s="258"/>
-      <c r="Y7" s="258"/>
-      <c r="Z7" s="258"/>
-      <c r="AA7" s="258"/>
-      <c r="AB7" s="258"/>
-      <c r="AC7" s="258"/>
-      <c r="AD7" s="258"/>
-      <c r="AE7" s="258"/>
-      <c r="AF7" s="258"/>
-      <c r="AG7" s="258"/>
-      <c r="AH7" s="258"/>
-      <c r="AI7" s="260" t="s">
+      <c r="R7" s="249"/>
+      <c r="S7" s="249"/>
+      <c r="T7" s="249"/>
+      <c r="U7" s="249"/>
+      <c r="V7" s="249"/>
+      <c r="W7" s="249"/>
+      <c r="X7" s="249"/>
+      <c r="Y7" s="249"/>
+      <c r="Z7" s="249"/>
+      <c r="AA7" s="249"/>
+      <c r="AB7" s="249"/>
+      <c r="AC7" s="249"/>
+      <c r="AD7" s="249"/>
+      <c r="AE7" s="249"/>
+      <c r="AF7" s="249"/>
+      <c r="AG7" s="249"/>
+      <c r="AH7" s="249"/>
+      <c r="AI7" s="215" t="s">
         <v>822</v>
       </c>
-      <c r="AJ7" s="260"/>
-      <c r="AK7" s="260"/>
-      <c r="AL7" s="260"/>
-      <c r="AM7" s="262" t="s">
+      <c r="AJ7" s="215"/>
+      <c r="AK7" s="215"/>
+      <c r="AL7" s="215"/>
+      <c r="AM7" s="217" t="s">
         <v>816</v>
       </c>
-      <c r="AN7" s="262"/>
-      <c r="AO7" s="262"/>
-      <c r="AP7" s="262"/>
-      <c r="AQ7" s="262"/>
-      <c r="AR7" s="262"/>
-      <c r="AS7" s="262"/>
-      <c r="AT7" s="264" t="s">
+      <c r="AN7" s="217"/>
+      <c r="AO7" s="217"/>
+      <c r="AP7" s="217"/>
+      <c r="AQ7" s="217"/>
+      <c r="AR7" s="217"/>
+      <c r="AS7" s="217"/>
+      <c r="AT7" s="157" t="s">
         <v>817</v>
       </c>
-      <c r="AU7" s="264"/>
-      <c r="AV7" s="264"/>
-      <c r="AW7" s="264"/>
-      <c r="AX7" s="264"/>
-      <c r="AY7" s="264"/>
-      <c r="AZ7" s="264"/>
-      <c r="BA7" s="266" t="s">
+      <c r="AU7" s="157"/>
+      <c r="AV7" s="157"/>
+      <c r="AW7" s="157"/>
+      <c r="AX7" s="157"/>
+      <c r="AY7" s="157"/>
+      <c r="AZ7" s="157"/>
+      <c r="BA7" s="219" t="s">
         <v>818</v>
       </c>
-      <c r="BB7" s="266"/>
-      <c r="BC7" s="266"/>
-      <c r="BD7" s="266"/>
-      <c r="BE7" s="266"/>
-      <c r="BF7" s="266"/>
-      <c r="BG7" s="266"/>
-      <c r="BH7" s="268" t="s">
+      <c r="BB7" s="219"/>
+      <c r="BC7" s="219"/>
+      <c r="BD7" s="219"/>
+      <c r="BE7" s="219"/>
+      <c r="BF7" s="219"/>
+      <c r="BG7" s="219"/>
+      <c r="BH7" s="221" t="s">
         <v>819</v>
       </c>
-      <c r="BI7" s="268"/>
-      <c r="BJ7" s="268"/>
-      <c r="BK7" s="268"/>
-      <c r="BL7" s="268"/>
-      <c r="BM7" s="268"/>
-      <c r="BN7" s="268"/>
-      <c r="BO7" s="169" t="s">
+      <c r="BI7" s="221"/>
+      <c r="BJ7" s="221"/>
+      <c r="BK7" s="221"/>
+      <c r="BL7" s="221"/>
+      <c r="BM7" s="221"/>
+      <c r="BN7" s="221"/>
+      <c r="BO7" s="253" t="s">
         <v>825</v>
       </c>
-      <c r="BP7" s="169"/>
-      <c r="BQ7" s="169"/>
-      <c r="BR7" s="169"/>
-      <c r="BS7" s="169"/>
-      <c r="BT7" s="169"/>
-      <c r="BU7" s="169"/>
-      <c r="BV7" s="169"/>
-      <c r="BW7" s="169"/>
-      <c r="BX7" s="169"/>
-      <c r="BY7" s="169"/>
-      <c r="BZ7" s="169"/>
-      <c r="CA7" s="169"/>
-      <c r="CB7" s="169"/>
-      <c r="CC7" s="169"/>
-      <c r="CD7" s="171" t="s">
+      <c r="BP7" s="253"/>
+      <c r="BQ7" s="253"/>
+      <c r="BR7" s="253"/>
+      <c r="BS7" s="253"/>
+      <c r="BT7" s="253"/>
+      <c r="BU7" s="253"/>
+      <c r="BV7" s="253"/>
+      <c r="BW7" s="253"/>
+      <c r="BX7" s="253"/>
+      <c r="BY7" s="253"/>
+      <c r="BZ7" s="253"/>
+      <c r="CA7" s="253"/>
+      <c r="CB7" s="253"/>
+      <c r="CC7" s="253"/>
+      <c r="CD7" s="266" t="s">
         <v>891</v>
       </c>
-      <c r="CE7" s="172"/>
-      <c r="CF7" s="172"/>
-      <c r="CG7" s="173"/>
+      <c r="CE7" s="267"/>
+      <c r="CF7" s="267"/>
+      <c r="CG7" s="268"/>
+      <c r="CH7" s="270"/>
     </row>
-    <row r="8" spans="1:85" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="253"/>
-      <c r="B8" s="254"/>
-      <c r="C8" s="254"/>
-      <c r="D8" s="254"/>
-      <c r="E8" s="254"/>
-      <c r="F8" s="254"/>
-      <c r="G8" s="254"/>
-      <c r="H8" s="254"/>
-      <c r="I8" s="254"/>
-      <c r="J8" s="254"/>
-      <c r="K8" s="255"/>
-      <c r="L8" s="257"/>
-      <c r="M8" s="257"/>
-      <c r="N8" s="257"/>
-      <c r="O8" s="257"/>
-      <c r="P8" s="257"/>
-      <c r="Q8" s="259"/>
-      <c r="R8" s="259"/>
-      <c r="S8" s="259"/>
-      <c r="T8" s="259"/>
-      <c r="U8" s="259"/>
-      <c r="V8" s="259"/>
-      <c r="W8" s="259"/>
-      <c r="X8" s="259"/>
-      <c r="Y8" s="259"/>
-      <c r="Z8" s="259"/>
-      <c r="AA8" s="259"/>
-      <c r="AB8" s="259"/>
-      <c r="AC8" s="259"/>
-      <c r="AD8" s="259"/>
-      <c r="AE8" s="259"/>
-      <c r="AF8" s="259"/>
-      <c r="AG8" s="259"/>
-      <c r="AH8" s="259"/>
-      <c r="AI8" s="261"/>
-      <c r="AJ8" s="261"/>
-      <c r="AK8" s="261"/>
-      <c r="AL8" s="261"/>
-      <c r="AM8" s="263"/>
-      <c r="AN8" s="263"/>
-      <c r="AO8" s="263"/>
-      <c r="AP8" s="263"/>
-      <c r="AQ8" s="263"/>
-      <c r="AR8" s="263"/>
-      <c r="AS8" s="263"/>
-      <c r="AT8" s="265"/>
-      <c r="AU8" s="265"/>
-      <c r="AV8" s="265"/>
-      <c r="AW8" s="265"/>
-      <c r="AX8" s="265"/>
-      <c r="AY8" s="265"/>
-      <c r="AZ8" s="265"/>
-      <c r="BA8" s="267"/>
-      <c r="BB8" s="267"/>
-      <c r="BC8" s="267"/>
-      <c r="BD8" s="267"/>
-      <c r="BE8" s="267"/>
-      <c r="BF8" s="267"/>
-      <c r="BG8" s="267"/>
-      <c r="BH8" s="269"/>
-      <c r="BI8" s="269"/>
-      <c r="BJ8" s="269"/>
-      <c r="BK8" s="269"/>
-      <c r="BL8" s="269"/>
-      <c r="BM8" s="269"/>
-      <c r="BN8" s="269"/>
-      <c r="BO8" s="170"/>
-      <c r="BP8" s="170"/>
-      <c r="BQ8" s="170"/>
-      <c r="BR8" s="170"/>
-      <c r="BS8" s="170"/>
-      <c r="BT8" s="170"/>
-      <c r="BU8" s="170"/>
-      <c r="BV8" s="170"/>
-      <c r="BW8" s="170"/>
-      <c r="BX8" s="170"/>
-      <c r="BY8" s="170"/>
-      <c r="BZ8" s="170"/>
-      <c r="CA8" s="170"/>
-      <c r="CB8" s="170"/>
-      <c r="CC8" s="170"/>
-      <c r="CD8" s="162"/>
-      <c r="CE8" s="163"/>
-      <c r="CF8" s="163"/>
-      <c r="CG8" s="164"/>
+    <row r="8" spans="1:86" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="244"/>
+      <c r="B8" s="245"/>
+      <c r="C8" s="245"/>
+      <c r="D8" s="245"/>
+      <c r="E8" s="245"/>
+      <c r="F8" s="245"/>
+      <c r="G8" s="245"/>
+      <c r="H8" s="245"/>
+      <c r="I8" s="245"/>
+      <c r="J8" s="245"/>
+      <c r="K8" s="246"/>
+      <c r="L8" s="248"/>
+      <c r="M8" s="248"/>
+      <c r="N8" s="248"/>
+      <c r="O8" s="248"/>
+      <c r="P8" s="248"/>
+      <c r="Q8" s="250"/>
+      <c r="R8" s="250"/>
+      <c r="S8" s="250"/>
+      <c r="T8" s="250"/>
+      <c r="U8" s="250"/>
+      <c r="V8" s="250"/>
+      <c r="W8" s="250"/>
+      <c r="X8" s="250"/>
+      <c r="Y8" s="250"/>
+      <c r="Z8" s="250"/>
+      <c r="AA8" s="250"/>
+      <c r="AB8" s="250"/>
+      <c r="AC8" s="250"/>
+      <c r="AD8" s="250"/>
+      <c r="AE8" s="250"/>
+      <c r="AF8" s="250"/>
+      <c r="AG8" s="250"/>
+      <c r="AH8" s="250"/>
+      <c r="AI8" s="216"/>
+      <c r="AJ8" s="216"/>
+      <c r="AK8" s="216"/>
+      <c r="AL8" s="216"/>
+      <c r="AM8" s="218"/>
+      <c r="AN8" s="218"/>
+      <c r="AO8" s="218"/>
+      <c r="AP8" s="218"/>
+      <c r="AQ8" s="218"/>
+      <c r="AR8" s="218"/>
+      <c r="AS8" s="218"/>
+      <c r="AT8" s="158"/>
+      <c r="AU8" s="158"/>
+      <c r="AV8" s="158"/>
+      <c r="AW8" s="158"/>
+      <c r="AX8" s="158"/>
+      <c r="AY8" s="158"/>
+      <c r="AZ8" s="158"/>
+      <c r="BA8" s="220"/>
+      <c r="BB8" s="220"/>
+      <c r="BC8" s="220"/>
+      <c r="BD8" s="220"/>
+      <c r="BE8" s="220"/>
+      <c r="BF8" s="220"/>
+      <c r="BG8" s="220"/>
+      <c r="BH8" s="222"/>
+      <c r="BI8" s="222"/>
+      <c r="BJ8" s="222"/>
+      <c r="BK8" s="222"/>
+      <c r="BL8" s="222"/>
+      <c r="BM8" s="222"/>
+      <c r="BN8" s="222"/>
+      <c r="BO8" s="254"/>
+      <c r="BP8" s="254"/>
+      <c r="BQ8" s="254"/>
+      <c r="BR8" s="254"/>
+      <c r="BS8" s="254"/>
+      <c r="BT8" s="254"/>
+      <c r="BU8" s="254"/>
+      <c r="BV8" s="254"/>
+      <c r="BW8" s="254"/>
+      <c r="BX8" s="254"/>
+      <c r="BY8" s="254"/>
+      <c r="BZ8" s="254"/>
+      <c r="CA8" s="254"/>
+      <c r="CB8" s="254"/>
+      <c r="CC8" s="254"/>
+      <c r="CD8" s="263"/>
+      <c r="CE8" s="264"/>
+      <c r="CF8" s="264"/>
+      <c r="CG8" s="265"/>
+      <c r="CH8" s="270"/>
     </row>
-    <row r="9" spans="1:85" s="29" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="226" t="s">
+    <row r="9" spans="1:86" s="29" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="223" t="s">
         <v>808</v>
       </c>
-      <c r="B9" s="228" t="s">
+      <c r="B9" s="225" t="s">
         <v>809</v>
       </c>
-      <c r="C9" s="228" t="s">
+      <c r="C9" s="225" t="s">
         <v>801</v>
       </c>
-      <c r="D9" s="228" t="s">
+      <c r="D9" s="225" t="s">
         <v>800</v>
       </c>
-      <c r="E9" s="228" t="s">
+      <c r="E9" s="225" t="s">
         <v>807</v>
       </c>
-      <c r="F9" s="228" t="s">
+      <c r="F9" s="225" t="s">
         <v>804</v>
       </c>
-      <c r="G9" s="228" t="s">
+      <c r="G9" s="225" t="s">
         <v>826</v>
       </c>
-      <c r="H9" s="228" t="s">
+      <c r="H9" s="225" t="s">
         <v>803</v>
       </c>
-      <c r="I9" s="240" t="s">
+      <c r="I9" s="227" t="s">
         <v>802</v>
       </c>
-      <c r="J9" s="228" t="s">
+      <c r="J9" s="225" t="s">
         <v>827</v>
       </c>
-      <c r="K9" s="234" t="s">
+      <c r="K9" s="229" t="s">
         <v>820</v>
       </c>
-      <c r="L9" s="236" t="s">
+      <c r="L9" s="231" t="s">
         <v>811</v>
       </c>
-      <c r="M9" s="214" t="s">
+      <c r="M9" s="175" t="s">
         <v>812</v>
       </c>
-      <c r="N9" s="214" t="s">
+      <c r="N9" s="175" t="s">
         <v>813</v>
       </c>
-      <c r="O9" s="238" t="s">
+      <c r="O9" s="233" t="s">
         <v>814</v>
       </c>
-      <c r="P9" s="230" t="s">
+      <c r="P9" s="235" t="s">
         <v>815</v>
       </c>
-      <c r="Q9" s="232" t="s">
+      <c r="Q9" s="237" t="s">
         <v>669</v>
       </c>
-      <c r="R9" s="193" t="s">
+      <c r="R9" s="239" t="s">
         <v>670</v>
       </c>
-      <c r="S9" s="193" t="s">
+      <c r="S9" s="239" t="s">
         <v>824</v>
       </c>
-      <c r="T9" s="193" t="s">
+      <c r="T9" s="239" t="s">
         <v>828</v>
       </c>
-      <c r="U9" s="193" t="s">
+      <c r="U9" s="239" t="s">
         <v>866</v>
       </c>
-      <c r="V9" s="242" t="s">
+      <c r="V9" s="251" t="s">
         <v>823</v>
       </c>
-      <c r="W9" s="193" t="s">
+      <c r="W9" s="239" t="s">
         <v>867</v>
       </c>
-      <c r="X9" s="193" t="s">
+      <c r="X9" s="239" t="s">
         <v>868</v>
       </c>
-      <c r="Y9" s="193" t="s">
+      <c r="Y9" s="239" t="s">
         <v>869</v>
       </c>
-      <c r="Z9" s="193" t="s">
+      <c r="Z9" s="239" t="s">
         <v>806</v>
       </c>
-      <c r="AA9" s="193" t="s">
+      <c r="AA9" s="239" t="s">
         <v>870</v>
       </c>
-      <c r="AB9" s="193" t="s">
+      <c r="AB9" s="239" t="s">
         <v>871</v>
       </c>
-      <c r="AC9" s="193" t="s">
+      <c r="AC9" s="239" t="s">
         <v>872</v>
       </c>
-      <c r="AD9" s="193" t="s">
+      <c r="AD9" s="239" t="s">
         <v>873</v>
       </c>
-      <c r="AE9" s="193" t="s">
+      <c r="AE9" s="239" t="s">
         <v>874</v>
       </c>
-      <c r="AF9" s="193" t="s">
+      <c r="AF9" s="239" t="s">
         <v>677</v>
       </c>
-      <c r="AG9" s="193" t="s">
+      <c r="AG9" s="239" t="s">
         <v>875</v>
       </c>
-      <c r="AH9" s="195" t="s">
+      <c r="AH9" s="201" t="s">
         <v>876</v>
       </c>
-      <c r="AI9" s="197" t="s">
+      <c r="AI9" s="203" t="s">
         <v>877</v>
       </c>
-      <c r="AJ9" s="244" t="s">
+      <c r="AJ9" s="205" t="s">
         <v>878</v>
       </c>
-      <c r="AK9" s="244" t="s">
+      <c r="AK9" s="205" t="s">
         <v>879</v>
       </c>
-      <c r="AL9" s="246" t="s">
+      <c r="AL9" s="207" t="s">
         <v>880</v>
       </c>
-      <c r="AM9" s="248" t="s">
+      <c r="AM9" s="209" t="s">
         <v>829</v>
       </c>
-      <c r="AN9" s="207" t="s">
+      <c r="AN9" s="211" t="s">
         <v>830</v>
       </c>
-      <c r="AO9" s="207" t="s">
+      <c r="AO9" s="211" t="s">
         <v>831</v>
       </c>
-      <c r="AP9" s="209" t="s">
+      <c r="AP9" s="213" t="s">
         <v>881</v>
       </c>
-      <c r="AQ9" s="210" t="s">
+      <c r="AQ9" s="179" t="s">
         <v>832</v>
       </c>
-      <c r="AR9" s="210" t="s">
+      <c r="AR9" s="179" t="s">
         <v>833</v>
       </c>
-      <c r="AS9" s="212" t="s">
+      <c r="AS9" s="181" t="s">
         <v>834</v>
       </c>
-      <c r="AT9" s="199" t="s">
+      <c r="AT9" s="159" t="s">
         <v>835</v>
       </c>
-      <c r="AU9" s="201" t="s">
+      <c r="AU9" s="161" t="s">
         <v>836</v>
       </c>
-      <c r="AV9" s="201" t="s">
+      <c r="AV9" s="161" t="s">
         <v>837</v>
       </c>
-      <c r="AW9" s="205" t="s">
+      <c r="AW9" s="163" t="s">
         <v>888</v>
       </c>
-      <c r="AX9" s="185" t="s">
+      <c r="AX9" s="165" t="s">
         <v>838</v>
       </c>
-      <c r="AY9" s="185" t="s">
+      <c r="AY9" s="165" t="s">
         <v>839</v>
       </c>
-      <c r="AZ9" s="187" t="s">
+      <c r="AZ9" s="167" t="s">
         <v>840</v>
       </c>
-      <c r="BA9" s="189" t="s">
+      <c r="BA9" s="171" t="s">
         <v>841</v>
       </c>
-      <c r="BB9" s="191" t="s">
+      <c r="BB9" s="177" t="s">
         <v>842</v>
       </c>
-      <c r="BC9" s="191" t="s">
+      <c r="BC9" s="177" t="s">
         <v>843</v>
       </c>
-      <c r="BD9" s="214" t="s">
+      <c r="BD9" s="175" t="s">
         <v>889</v>
       </c>
-      <c r="BE9" s="216" t="s">
+      <c r="BE9" s="173" t="s">
         <v>844</v>
       </c>
-      <c r="BF9" s="216" t="s">
+      <c r="BF9" s="173" t="s">
         <v>845</v>
       </c>
-      <c r="BG9" s="224" t="s">
+      <c r="BG9" s="169" t="s">
         <v>846</v>
       </c>
-      <c r="BH9" s="183" t="s">
+      <c r="BH9" s="255" t="s">
         <v>847</v>
       </c>
-      <c r="BI9" s="218" t="s">
+      <c r="BI9" s="199" t="s">
         <v>848</v>
       </c>
-      <c r="BJ9" s="218" t="s">
+      <c r="BJ9" s="199" t="s">
         <v>849</v>
       </c>
-      <c r="BK9" s="220" t="s">
+      <c r="BK9" s="197" t="s">
         <v>890</v>
       </c>
-      <c r="BL9" s="222" t="s">
+      <c r="BL9" s="193" t="s">
         <v>850</v>
       </c>
-      <c r="BM9" s="222" t="s">
+      <c r="BM9" s="193" t="s">
         <v>851</v>
       </c>
-      <c r="BN9" s="203" t="s">
+      <c r="BN9" s="195" t="s">
         <v>852</v>
       </c>
-      <c r="BO9" s="177" t="s">
+      <c r="BO9" s="191" t="s">
         <v>853</v>
       </c>
-      <c r="BP9" s="179" t="s">
+      <c r="BP9" s="187" t="s">
         <v>854</v>
       </c>
-      <c r="BQ9" s="181" t="s">
+      <c r="BQ9" s="189" t="s">
         <v>855</v>
       </c>
-      <c r="BR9" s="181" t="s">
+      <c r="BR9" s="189" t="s">
         <v>856</v>
       </c>
-      <c r="BS9" s="167" t="s">
+      <c r="BS9" s="185" t="s">
         <v>857</v>
       </c>
-      <c r="BT9" s="179" t="s">
+      <c r="BT9" s="187" t="s">
         <v>858</v>
       </c>
-      <c r="BU9" s="167" t="s">
+      <c r="BU9" s="185" t="s">
         <v>755</v>
       </c>
-      <c r="BV9" s="167" t="s">
+      <c r="BV9" s="185" t="s">
         <v>766</v>
       </c>
-      <c r="BW9" s="167" t="s">
+      <c r="BW9" s="185" t="s">
         <v>859</v>
       </c>
-      <c r="BX9" s="167" t="s">
+      <c r="BX9" s="185" t="s">
         <v>860</v>
       </c>
-      <c r="BY9" s="167" t="s">
+      <c r="BY9" s="185" t="s">
         <v>861</v>
       </c>
-      <c r="BZ9" s="167" t="s">
+      <c r="BZ9" s="185" t="s">
         <v>862</v>
       </c>
-      <c r="CA9" s="167" t="s">
+      <c r="CA9" s="185" t="s">
         <v>863</v>
       </c>
-      <c r="CB9" s="167" t="s">
+      <c r="CB9" s="185" t="s">
         <v>864</v>
       </c>
-      <c r="CC9" s="165" t="s">
+      <c r="CC9" s="183" t="s">
         <v>865</v>
       </c>
-      <c r="CD9" s="174" t="s">
+      <c r="CD9" s="214" t="s">
         <v>892</v>
       </c>
-      <c r="CE9" s="174" t="s">
+      <c r="CE9" s="214" t="s">
         <v>895</v>
       </c>
-      <c r="CF9" s="174" t="s">
+      <c r="CF9" s="214" t="s">
         <v>893</v>
       </c>
-      <c r="CG9" s="176" t="s">
+      <c r="CG9" s="269" t="s">
         <v>894</v>
       </c>
+      <c r="CH9" s="271" t="s">
+        <v>896</v>
+      </c>
     </row>
-    <row r="10" spans="1:85" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="227"/>
-      <c r="B10" s="229"/>
-      <c r="C10" s="229"/>
-      <c r="D10" s="229"/>
-      <c r="E10" s="229"/>
-      <c r="F10" s="229"/>
-      <c r="G10" s="229"/>
-      <c r="H10" s="229"/>
-      <c r="I10" s="241"/>
-      <c r="J10" s="229"/>
-      <c r="K10" s="235"/>
-      <c r="L10" s="237"/>
-      <c r="M10" s="215"/>
-      <c r="N10" s="215"/>
-      <c r="O10" s="239"/>
-      <c r="P10" s="231"/>
-      <c r="Q10" s="233"/>
-      <c r="R10" s="194"/>
-      <c r="S10" s="194"/>
-      <c r="T10" s="194"/>
-      <c r="U10" s="194"/>
-      <c r="V10" s="243"/>
-      <c r="W10" s="194"/>
-      <c r="X10" s="194"/>
-      <c r="Y10" s="194"/>
-      <c r="Z10" s="194"/>
-      <c r="AA10" s="194"/>
-      <c r="AB10" s="194"/>
-      <c r="AC10" s="194"/>
-      <c r="AD10" s="194"/>
-      <c r="AE10" s="194"/>
-      <c r="AF10" s="194"/>
-      <c r="AG10" s="194"/>
-      <c r="AH10" s="196"/>
-      <c r="AI10" s="198"/>
-      <c r="AJ10" s="245"/>
-      <c r="AK10" s="245"/>
-      <c r="AL10" s="247"/>
-      <c r="AM10" s="249"/>
-      <c r="AN10" s="208"/>
-      <c r="AO10" s="208"/>
-      <c r="AP10" s="174"/>
-      <c r="AQ10" s="211"/>
-      <c r="AR10" s="211"/>
-      <c r="AS10" s="213"/>
-      <c r="AT10" s="200"/>
-      <c r="AU10" s="202"/>
-      <c r="AV10" s="202"/>
-      <c r="AW10" s="206"/>
-      <c r="AX10" s="186"/>
-      <c r="AY10" s="186"/>
-      <c r="AZ10" s="188"/>
-      <c r="BA10" s="190"/>
-      <c r="BB10" s="192"/>
-      <c r="BC10" s="192"/>
-      <c r="BD10" s="215"/>
-      <c r="BE10" s="217"/>
-      <c r="BF10" s="217"/>
-      <c r="BG10" s="225"/>
-      <c r="BH10" s="184"/>
-      <c r="BI10" s="219"/>
-      <c r="BJ10" s="219"/>
-      <c r="BK10" s="221"/>
-      <c r="BL10" s="223"/>
-      <c r="BM10" s="223"/>
-      <c r="BN10" s="204"/>
-      <c r="BO10" s="178"/>
-      <c r="BP10" s="180"/>
-      <c r="BQ10" s="182"/>
-      <c r="BR10" s="182"/>
-      <c r="BS10" s="168"/>
-      <c r="BT10" s="180"/>
-      <c r="BU10" s="168"/>
-      <c r="BV10" s="168"/>
-      <c r="BW10" s="168"/>
-      <c r="BX10" s="168"/>
-      <c r="BY10" s="168"/>
-      <c r="BZ10" s="168"/>
-      <c r="CA10" s="168"/>
-      <c r="CB10" s="168"/>
-      <c r="CC10" s="166"/>
-      <c r="CD10" s="175"/>
-      <c r="CE10" s="175"/>
-      <c r="CF10" s="175"/>
-      <c r="CG10" s="158"/>
+    <row r="10" spans="1:86" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="224"/>
+      <c r="B10" s="226"/>
+      <c r="C10" s="226"/>
+      <c r="D10" s="226"/>
+      <c r="E10" s="226"/>
+      <c r="F10" s="226"/>
+      <c r="G10" s="226"/>
+      <c r="H10" s="226"/>
+      <c r="I10" s="228"/>
+      <c r="J10" s="226"/>
+      <c r="K10" s="230"/>
+      <c r="L10" s="232"/>
+      <c r="M10" s="176"/>
+      <c r="N10" s="176"/>
+      <c r="O10" s="234"/>
+      <c r="P10" s="236"/>
+      <c r="Q10" s="238"/>
+      <c r="R10" s="240"/>
+      <c r="S10" s="240"/>
+      <c r="T10" s="240"/>
+      <c r="U10" s="240"/>
+      <c r="V10" s="252"/>
+      <c r="W10" s="240"/>
+      <c r="X10" s="240"/>
+      <c r="Y10" s="240"/>
+      <c r="Z10" s="240"/>
+      <c r="AA10" s="240"/>
+      <c r="AB10" s="240"/>
+      <c r="AC10" s="240"/>
+      <c r="AD10" s="240"/>
+      <c r="AE10" s="240"/>
+      <c r="AF10" s="240"/>
+      <c r="AG10" s="240"/>
+      <c r="AH10" s="202"/>
+      <c r="AI10" s="204"/>
+      <c r="AJ10" s="206"/>
+      <c r="AK10" s="206"/>
+      <c r="AL10" s="208"/>
+      <c r="AM10" s="210"/>
+      <c r="AN10" s="212"/>
+      <c r="AO10" s="212"/>
+      <c r="AP10" s="214"/>
+      <c r="AQ10" s="180"/>
+      <c r="AR10" s="180"/>
+      <c r="AS10" s="182"/>
+      <c r="AT10" s="160"/>
+      <c r="AU10" s="162"/>
+      <c r="AV10" s="162"/>
+      <c r="AW10" s="164"/>
+      <c r="AX10" s="166"/>
+      <c r="AY10" s="166"/>
+      <c r="AZ10" s="168"/>
+      <c r="BA10" s="172"/>
+      <c r="BB10" s="178"/>
+      <c r="BC10" s="178"/>
+      <c r="BD10" s="176"/>
+      <c r="BE10" s="174"/>
+      <c r="BF10" s="174"/>
+      <c r="BG10" s="170"/>
+      <c r="BH10" s="256"/>
+      <c r="BI10" s="200"/>
+      <c r="BJ10" s="200"/>
+      <c r="BK10" s="198"/>
+      <c r="BL10" s="194"/>
+      <c r="BM10" s="194"/>
+      <c r="BN10" s="196"/>
+      <c r="BO10" s="192"/>
+      <c r="BP10" s="188"/>
+      <c r="BQ10" s="190"/>
+      <c r="BR10" s="190"/>
+      <c r="BS10" s="186"/>
+      <c r="BT10" s="188"/>
+      <c r="BU10" s="186"/>
+      <c r="BV10" s="186"/>
+      <c r="BW10" s="186"/>
+      <c r="BX10" s="186"/>
+      <c r="BY10" s="186"/>
+      <c r="BZ10" s="186"/>
+      <c r="CA10" s="186"/>
+      <c r="CB10" s="186"/>
+      <c r="CC10" s="184"/>
+      <c r="CD10" s="257"/>
+      <c r="CE10" s="257"/>
+      <c r="CF10" s="257"/>
+      <c r="CG10" s="259"/>
+      <c r="CH10" s="272"/>
     </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -15075,8 +15108,9 @@
       <c r="CE11" s="155"/>
       <c r="CF11" s="155"/>
       <c r="CG11" s="156"/>
+      <c r="CH11" s="274"/>
     </row>
-    <row r="12" spans="1:85" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:86" ht="11" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -15166,547 +15200,554 @@
       <c r="CE12" s="74"/>
       <c r="CF12" s="74"/>
       <c r="CG12" s="153"/>
+      <c r="CH12" s="273"/>
     </row>
-    <row r="13" spans="1:85" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:85" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="250" t="s">
+    <row r="13" spans="1:86" ht="11" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:86" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="241" t="s">
         <v>805</v>
       </c>
-      <c r="B14" s="251"/>
-      <c r="C14" s="251"/>
-      <c r="D14" s="251"/>
-      <c r="E14" s="251"/>
-      <c r="F14" s="251"/>
-      <c r="G14" s="251"/>
-      <c r="H14" s="251"/>
-      <c r="I14" s="251"/>
-      <c r="J14" s="251"/>
-      <c r="K14" s="252"/>
-      <c r="L14" s="256" t="s">
+      <c r="B14" s="242"/>
+      <c r="C14" s="242"/>
+      <c r="D14" s="242"/>
+      <c r="E14" s="242"/>
+      <c r="F14" s="242"/>
+      <c r="G14" s="242"/>
+      <c r="H14" s="242"/>
+      <c r="I14" s="242"/>
+      <c r="J14" s="242"/>
+      <c r="K14" s="243"/>
+      <c r="L14" s="247" t="s">
         <v>810</v>
       </c>
-      <c r="M14" s="256"/>
-      <c r="N14" s="256"/>
-      <c r="O14" s="256"/>
-      <c r="P14" s="256"/>
-      <c r="Q14" s="258" t="s">
+      <c r="M14" s="247"/>
+      <c r="N14" s="247"/>
+      <c r="O14" s="247"/>
+      <c r="P14" s="247"/>
+      <c r="Q14" s="249" t="s">
         <v>821</v>
       </c>
-      <c r="R14" s="258"/>
-      <c r="S14" s="258"/>
-      <c r="T14" s="258"/>
-      <c r="U14" s="258"/>
-      <c r="V14" s="258"/>
-      <c r="W14" s="258"/>
-      <c r="X14" s="258"/>
-      <c r="Y14" s="258"/>
-      <c r="Z14" s="258"/>
-      <c r="AA14" s="258"/>
-      <c r="AB14" s="258"/>
-      <c r="AC14" s="258"/>
-      <c r="AD14" s="258"/>
-      <c r="AE14" s="258"/>
-      <c r="AF14" s="258"/>
-      <c r="AG14" s="258"/>
-      <c r="AH14" s="258"/>
-      <c r="AI14" s="260" t="s">
+      <c r="R14" s="249"/>
+      <c r="S14" s="249"/>
+      <c r="T14" s="249"/>
+      <c r="U14" s="249"/>
+      <c r="V14" s="249"/>
+      <c r="W14" s="249"/>
+      <c r="X14" s="249"/>
+      <c r="Y14" s="249"/>
+      <c r="Z14" s="249"/>
+      <c r="AA14" s="249"/>
+      <c r="AB14" s="249"/>
+      <c r="AC14" s="249"/>
+      <c r="AD14" s="249"/>
+      <c r="AE14" s="249"/>
+      <c r="AF14" s="249"/>
+      <c r="AG14" s="249"/>
+      <c r="AH14" s="249"/>
+      <c r="AI14" s="215" t="s">
         <v>822</v>
       </c>
-      <c r="AJ14" s="260"/>
-      <c r="AK14" s="260"/>
-      <c r="AL14" s="260"/>
-      <c r="AM14" s="262" t="s">
+      <c r="AJ14" s="215"/>
+      <c r="AK14" s="215"/>
+      <c r="AL14" s="215"/>
+      <c r="AM14" s="217" t="s">
         <v>816</v>
       </c>
-      <c r="AN14" s="262"/>
-      <c r="AO14" s="262"/>
-      <c r="AP14" s="262"/>
-      <c r="AQ14" s="262"/>
-      <c r="AR14" s="262"/>
-      <c r="AS14" s="262"/>
-      <c r="AT14" s="264" t="s">
+      <c r="AN14" s="217"/>
+      <c r="AO14" s="217"/>
+      <c r="AP14" s="217"/>
+      <c r="AQ14" s="217"/>
+      <c r="AR14" s="217"/>
+      <c r="AS14" s="217"/>
+      <c r="AT14" s="157" t="s">
         <v>817</v>
       </c>
-      <c r="AU14" s="264"/>
-      <c r="AV14" s="264"/>
-      <c r="AW14" s="264"/>
-      <c r="AX14" s="264"/>
-      <c r="AY14" s="264"/>
-      <c r="AZ14" s="264"/>
-      <c r="BA14" s="266" t="s">
+      <c r="AU14" s="157"/>
+      <c r="AV14" s="157"/>
+      <c r="AW14" s="157"/>
+      <c r="AX14" s="157"/>
+      <c r="AY14" s="157"/>
+      <c r="AZ14" s="157"/>
+      <c r="BA14" s="219" t="s">
         <v>818</v>
       </c>
-      <c r="BB14" s="266"/>
-      <c r="BC14" s="266"/>
-      <c r="BD14" s="266"/>
-      <c r="BE14" s="266"/>
-      <c r="BF14" s="266"/>
-      <c r="BG14" s="266"/>
-      <c r="BH14" s="268" t="s">
+      <c r="BB14" s="219"/>
+      <c r="BC14" s="219"/>
+      <c r="BD14" s="219"/>
+      <c r="BE14" s="219"/>
+      <c r="BF14" s="219"/>
+      <c r="BG14" s="219"/>
+      <c r="BH14" s="221" t="s">
         <v>819</v>
       </c>
-      <c r="BI14" s="268"/>
-      <c r="BJ14" s="268"/>
-      <c r="BK14" s="268"/>
-      <c r="BL14" s="268"/>
-      <c r="BM14" s="268"/>
-      <c r="BN14" s="268"/>
-      <c r="BO14" s="169" t="s">
+      <c r="BI14" s="221"/>
+      <c r="BJ14" s="221"/>
+      <c r="BK14" s="221"/>
+      <c r="BL14" s="221"/>
+      <c r="BM14" s="221"/>
+      <c r="BN14" s="221"/>
+      <c r="BO14" s="253" t="s">
         <v>825</v>
       </c>
-      <c r="BP14" s="169"/>
-      <c r="BQ14" s="169"/>
-      <c r="BR14" s="169"/>
-      <c r="BS14" s="169"/>
-      <c r="BT14" s="169"/>
-      <c r="BU14" s="169"/>
-      <c r="BV14" s="169"/>
-      <c r="BW14" s="169"/>
-      <c r="BX14" s="169"/>
-      <c r="BY14" s="169"/>
-      <c r="BZ14" s="169"/>
-      <c r="CA14" s="169"/>
-      <c r="CB14" s="169"/>
-      <c r="CC14" s="169"/>
-      <c r="CD14" s="171" t="s">
+      <c r="BP14" s="253"/>
+      <c r="BQ14" s="253"/>
+      <c r="BR14" s="253"/>
+      <c r="BS14" s="253"/>
+      <c r="BT14" s="253"/>
+      <c r="BU14" s="253"/>
+      <c r="BV14" s="253"/>
+      <c r="BW14" s="253"/>
+      <c r="BX14" s="253"/>
+      <c r="BY14" s="253"/>
+      <c r="BZ14" s="253"/>
+      <c r="CA14" s="253"/>
+      <c r="CB14" s="253"/>
+      <c r="CC14" s="253"/>
+      <c r="CD14" s="266" t="s">
         <v>891</v>
       </c>
-      <c r="CE14" s="172"/>
-      <c r="CF14" s="172"/>
-      <c r="CG14" s="173"/>
+      <c r="CE14" s="267"/>
+      <c r="CF14" s="267"/>
+      <c r="CG14" s="268"/>
+      <c r="CH14" s="270"/>
     </row>
-    <row r="15" spans="1:85" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="253"/>
-      <c r="B15" s="254"/>
-      <c r="C15" s="254"/>
-      <c r="D15" s="254"/>
-      <c r="E15" s="254"/>
-      <c r="F15" s="254"/>
-      <c r="G15" s="254"/>
-      <c r="H15" s="254"/>
-      <c r="I15" s="254"/>
-      <c r="J15" s="254"/>
-      <c r="K15" s="255"/>
-      <c r="L15" s="257"/>
-      <c r="M15" s="257"/>
-      <c r="N15" s="257"/>
-      <c r="O15" s="257"/>
-      <c r="P15" s="257"/>
-      <c r="Q15" s="259"/>
-      <c r="R15" s="259"/>
-      <c r="S15" s="259"/>
-      <c r="T15" s="259"/>
-      <c r="U15" s="259"/>
-      <c r="V15" s="259"/>
-      <c r="W15" s="259"/>
-      <c r="X15" s="259"/>
-      <c r="Y15" s="259"/>
-      <c r="Z15" s="259"/>
-      <c r="AA15" s="259"/>
-      <c r="AB15" s="259"/>
-      <c r="AC15" s="259"/>
-      <c r="AD15" s="259"/>
-      <c r="AE15" s="259"/>
-      <c r="AF15" s="259"/>
-      <c r="AG15" s="259"/>
-      <c r="AH15" s="259"/>
-      <c r="AI15" s="261"/>
-      <c r="AJ15" s="261"/>
-      <c r="AK15" s="261"/>
-      <c r="AL15" s="261"/>
-      <c r="AM15" s="263"/>
-      <c r="AN15" s="263"/>
-      <c r="AO15" s="263"/>
-      <c r="AP15" s="263"/>
-      <c r="AQ15" s="263"/>
-      <c r="AR15" s="263"/>
-      <c r="AS15" s="263"/>
-      <c r="AT15" s="265"/>
-      <c r="AU15" s="265"/>
-      <c r="AV15" s="265"/>
-      <c r="AW15" s="265"/>
-      <c r="AX15" s="265"/>
-      <c r="AY15" s="265"/>
-      <c r="AZ15" s="265"/>
-      <c r="BA15" s="267"/>
-      <c r="BB15" s="267"/>
-      <c r="BC15" s="267"/>
-      <c r="BD15" s="267"/>
-      <c r="BE15" s="267"/>
-      <c r="BF15" s="267"/>
-      <c r="BG15" s="267"/>
-      <c r="BH15" s="269"/>
-      <c r="BI15" s="269"/>
-      <c r="BJ15" s="269"/>
-      <c r="BK15" s="269"/>
-      <c r="BL15" s="269"/>
-      <c r="BM15" s="269"/>
-      <c r="BN15" s="269"/>
-      <c r="BO15" s="170"/>
-      <c r="BP15" s="170"/>
-      <c r="BQ15" s="170"/>
-      <c r="BR15" s="170"/>
-      <c r="BS15" s="170"/>
-      <c r="BT15" s="170"/>
-      <c r="BU15" s="170"/>
-      <c r="BV15" s="170"/>
-      <c r="BW15" s="170"/>
-      <c r="BX15" s="170"/>
-      <c r="BY15" s="170"/>
-      <c r="BZ15" s="170"/>
-      <c r="CA15" s="170"/>
-      <c r="CB15" s="170"/>
-      <c r="CC15" s="170"/>
-      <c r="CD15" s="162"/>
-      <c r="CE15" s="163"/>
-      <c r="CF15" s="163"/>
-      <c r="CG15" s="164"/>
+    <row r="15" spans="1:86" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="244"/>
+      <c r="B15" s="245"/>
+      <c r="C15" s="245"/>
+      <c r="D15" s="245"/>
+      <c r="E15" s="245"/>
+      <c r="F15" s="245"/>
+      <c r="G15" s="245"/>
+      <c r="H15" s="245"/>
+      <c r="I15" s="245"/>
+      <c r="J15" s="245"/>
+      <c r="K15" s="246"/>
+      <c r="L15" s="248"/>
+      <c r="M15" s="248"/>
+      <c r="N15" s="248"/>
+      <c r="O15" s="248"/>
+      <c r="P15" s="248"/>
+      <c r="Q15" s="250"/>
+      <c r="R15" s="250"/>
+      <c r="S15" s="250"/>
+      <c r="T15" s="250"/>
+      <c r="U15" s="250"/>
+      <c r="V15" s="250"/>
+      <c r="W15" s="250"/>
+      <c r="X15" s="250"/>
+      <c r="Y15" s="250"/>
+      <c r="Z15" s="250"/>
+      <c r="AA15" s="250"/>
+      <c r="AB15" s="250"/>
+      <c r="AC15" s="250"/>
+      <c r="AD15" s="250"/>
+      <c r="AE15" s="250"/>
+      <c r="AF15" s="250"/>
+      <c r="AG15" s="250"/>
+      <c r="AH15" s="250"/>
+      <c r="AI15" s="216"/>
+      <c r="AJ15" s="216"/>
+      <c r="AK15" s="216"/>
+      <c r="AL15" s="216"/>
+      <c r="AM15" s="218"/>
+      <c r="AN15" s="218"/>
+      <c r="AO15" s="218"/>
+      <c r="AP15" s="218"/>
+      <c r="AQ15" s="218"/>
+      <c r="AR15" s="218"/>
+      <c r="AS15" s="218"/>
+      <c r="AT15" s="158"/>
+      <c r="AU15" s="158"/>
+      <c r="AV15" s="158"/>
+      <c r="AW15" s="158"/>
+      <c r="AX15" s="158"/>
+      <c r="AY15" s="158"/>
+      <c r="AZ15" s="158"/>
+      <c r="BA15" s="220"/>
+      <c r="BB15" s="220"/>
+      <c r="BC15" s="220"/>
+      <c r="BD15" s="220"/>
+      <c r="BE15" s="220"/>
+      <c r="BF15" s="220"/>
+      <c r="BG15" s="220"/>
+      <c r="BH15" s="222"/>
+      <c r="BI15" s="222"/>
+      <c r="BJ15" s="222"/>
+      <c r="BK15" s="222"/>
+      <c r="BL15" s="222"/>
+      <c r="BM15" s="222"/>
+      <c r="BN15" s="222"/>
+      <c r="BO15" s="254"/>
+      <c r="BP15" s="254"/>
+      <c r="BQ15" s="254"/>
+      <c r="BR15" s="254"/>
+      <c r="BS15" s="254"/>
+      <c r="BT15" s="254"/>
+      <c r="BU15" s="254"/>
+      <c r="BV15" s="254"/>
+      <c r="BW15" s="254"/>
+      <c r="BX15" s="254"/>
+      <c r="BY15" s="254"/>
+      <c r="BZ15" s="254"/>
+      <c r="CA15" s="254"/>
+      <c r="CB15" s="254"/>
+      <c r="CC15" s="254"/>
+      <c r="CD15" s="263"/>
+      <c r="CE15" s="264"/>
+      <c r="CF15" s="264"/>
+      <c r="CG15" s="265"/>
+      <c r="CH15" s="270"/>
     </row>
-    <row r="16" spans="1:85" s="29" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="226" t="s">
+    <row r="16" spans="1:86" s="29" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="223" t="s">
         <v>808</v>
       </c>
-      <c r="B16" s="228" t="s">
+      <c r="B16" s="225" t="s">
         <v>809</v>
       </c>
-      <c r="C16" s="228" t="s">
+      <c r="C16" s="225" t="s">
         <v>801</v>
       </c>
-      <c r="D16" s="228" t="s">
+      <c r="D16" s="225" t="s">
         <v>800</v>
       </c>
-      <c r="E16" s="228" t="s">
+      <c r="E16" s="225" t="s">
         <v>807</v>
       </c>
-      <c r="F16" s="228" t="s">
+      <c r="F16" s="225" t="s">
         <v>804</v>
       </c>
-      <c r="G16" s="228" t="s">
+      <c r="G16" s="225" t="s">
         <v>826</v>
       </c>
-      <c r="H16" s="228" t="s">
+      <c r="H16" s="225" t="s">
         <v>803</v>
       </c>
-      <c r="I16" s="240" t="s">
+      <c r="I16" s="227" t="s">
         <v>802</v>
       </c>
-      <c r="J16" s="228" t="s">
+      <c r="J16" s="225" t="s">
         <v>827</v>
       </c>
-      <c r="K16" s="234" t="s">
+      <c r="K16" s="229" t="s">
         <v>820</v>
       </c>
-      <c r="L16" s="236" t="s">
+      <c r="L16" s="231" t="s">
         <v>811</v>
       </c>
-      <c r="M16" s="214" t="s">
+      <c r="M16" s="175" t="s">
         <v>812</v>
       </c>
-      <c r="N16" s="214" t="s">
+      <c r="N16" s="175" t="s">
         <v>813</v>
       </c>
-      <c r="O16" s="238" t="s">
+      <c r="O16" s="233" t="s">
         <v>814</v>
       </c>
-      <c r="P16" s="230" t="s">
+      <c r="P16" s="235" t="s">
         <v>815</v>
       </c>
-      <c r="Q16" s="232" t="s">
+      <c r="Q16" s="237" t="s">
         <v>669</v>
       </c>
-      <c r="R16" s="193" t="s">
+      <c r="R16" s="239" t="s">
         <v>670</v>
       </c>
-      <c r="S16" s="193" t="s">
+      <c r="S16" s="239" t="s">
         <v>824</v>
       </c>
-      <c r="T16" s="193" t="s">
+      <c r="T16" s="239" t="s">
         <v>828</v>
       </c>
-      <c r="U16" s="193" t="s">
+      <c r="U16" s="239" t="s">
         <v>866</v>
       </c>
-      <c r="V16" s="242" t="s">
+      <c r="V16" s="251" t="s">
         <v>823</v>
       </c>
-      <c r="W16" s="193" t="s">
+      <c r="W16" s="239" t="s">
         <v>867</v>
       </c>
-      <c r="X16" s="193" t="s">
+      <c r="X16" s="239" t="s">
         <v>868</v>
       </c>
-      <c r="Y16" s="193" t="s">
+      <c r="Y16" s="239" t="s">
         <v>869</v>
       </c>
-      <c r="Z16" s="193" t="s">
+      <c r="Z16" s="239" t="s">
         <v>806</v>
       </c>
-      <c r="AA16" s="193" t="s">
+      <c r="AA16" s="239" t="s">
         <v>870</v>
       </c>
-      <c r="AB16" s="193" t="s">
+      <c r="AB16" s="239" t="s">
         <v>871</v>
       </c>
-      <c r="AC16" s="193" t="s">
+      <c r="AC16" s="239" t="s">
         <v>872</v>
       </c>
-      <c r="AD16" s="193" t="s">
+      <c r="AD16" s="239" t="s">
         <v>873</v>
       </c>
-      <c r="AE16" s="193" t="s">
+      <c r="AE16" s="239" t="s">
         <v>874</v>
       </c>
-      <c r="AF16" s="193" t="s">
+      <c r="AF16" s="239" t="s">
         <v>677</v>
       </c>
-      <c r="AG16" s="193" t="s">
+      <c r="AG16" s="239" t="s">
         <v>875</v>
       </c>
-      <c r="AH16" s="195" t="s">
+      <c r="AH16" s="201" t="s">
         <v>876</v>
       </c>
-      <c r="AI16" s="197" t="s">
+      <c r="AI16" s="203" t="s">
         <v>877</v>
       </c>
-      <c r="AJ16" s="244" t="s">
+      <c r="AJ16" s="205" t="s">
         <v>878</v>
       </c>
-      <c r="AK16" s="244" t="s">
+      <c r="AK16" s="205" t="s">
         <v>879</v>
       </c>
-      <c r="AL16" s="246" t="s">
+      <c r="AL16" s="207" t="s">
         <v>880</v>
       </c>
-      <c r="AM16" s="248" t="s">
+      <c r="AM16" s="209" t="s">
         <v>829</v>
       </c>
-      <c r="AN16" s="207" t="s">
+      <c r="AN16" s="211" t="s">
         <v>830</v>
       </c>
-      <c r="AO16" s="207" t="s">
+      <c r="AO16" s="211" t="s">
         <v>831</v>
       </c>
-      <c r="AP16" s="209" t="s">
+      <c r="AP16" s="213" t="s">
         <v>881</v>
       </c>
-      <c r="AQ16" s="210" t="s">
+      <c r="AQ16" s="179" t="s">
         <v>832</v>
       </c>
-      <c r="AR16" s="210" t="s">
+      <c r="AR16" s="179" t="s">
         <v>833</v>
       </c>
-      <c r="AS16" s="212" t="s">
+      <c r="AS16" s="181" t="s">
         <v>834</v>
       </c>
-      <c r="AT16" s="199" t="s">
+      <c r="AT16" s="159" t="s">
         <v>835</v>
       </c>
-      <c r="AU16" s="201" t="s">
+      <c r="AU16" s="161" t="s">
         <v>836</v>
       </c>
-      <c r="AV16" s="201" t="s">
+      <c r="AV16" s="161" t="s">
         <v>837</v>
       </c>
-      <c r="AW16" s="205" t="s">
+      <c r="AW16" s="163" t="s">
         <v>888</v>
       </c>
-      <c r="AX16" s="185" t="s">
+      <c r="AX16" s="165" t="s">
         <v>838</v>
       </c>
-      <c r="AY16" s="185" t="s">
+      <c r="AY16" s="165" t="s">
         <v>839</v>
       </c>
-      <c r="AZ16" s="187" t="s">
+      <c r="AZ16" s="167" t="s">
         <v>840</v>
       </c>
-      <c r="BA16" s="189" t="s">
+      <c r="BA16" s="171" t="s">
         <v>841</v>
       </c>
-      <c r="BB16" s="191" t="s">
+      <c r="BB16" s="177" t="s">
         <v>842</v>
       </c>
-      <c r="BC16" s="191" t="s">
+      <c r="BC16" s="177" t="s">
         <v>843</v>
       </c>
-      <c r="BD16" s="214" t="s">
+      <c r="BD16" s="175" t="s">
         <v>889</v>
       </c>
-      <c r="BE16" s="216" t="s">
+      <c r="BE16" s="173" t="s">
         <v>844</v>
       </c>
-      <c r="BF16" s="216" t="s">
+      <c r="BF16" s="173" t="s">
         <v>845</v>
       </c>
-      <c r="BG16" s="224" t="s">
+      <c r="BG16" s="169" t="s">
         <v>846</v>
       </c>
-      <c r="BH16" s="183" t="s">
+      <c r="BH16" s="255" t="s">
         <v>847</v>
       </c>
-      <c r="BI16" s="218" t="s">
+      <c r="BI16" s="199" t="s">
         <v>848</v>
       </c>
-      <c r="BJ16" s="218" t="s">
+      <c r="BJ16" s="199" t="s">
         <v>849</v>
       </c>
-      <c r="BK16" s="220" t="s">
+      <c r="BK16" s="197" t="s">
         <v>890</v>
       </c>
-      <c r="BL16" s="222" t="s">
+      <c r="BL16" s="193" t="s">
         <v>850</v>
       </c>
-      <c r="BM16" s="222" t="s">
+      <c r="BM16" s="193" t="s">
         <v>851</v>
       </c>
-      <c r="BN16" s="203" t="s">
+      <c r="BN16" s="195" t="s">
         <v>852</v>
       </c>
-      <c r="BO16" s="177" t="s">
+      <c r="BO16" s="191" t="s">
         <v>853</v>
       </c>
-      <c r="BP16" s="179" t="s">
+      <c r="BP16" s="187" t="s">
         <v>854</v>
       </c>
-      <c r="BQ16" s="181" t="s">
+      <c r="BQ16" s="189" t="s">
         <v>855</v>
       </c>
-      <c r="BR16" s="181" t="s">
+      <c r="BR16" s="189" t="s">
         <v>856</v>
       </c>
-      <c r="BS16" s="167" t="s">
+      <c r="BS16" s="185" t="s">
         <v>857</v>
       </c>
-      <c r="BT16" s="179" t="s">
+      <c r="BT16" s="187" t="s">
         <v>858</v>
       </c>
-      <c r="BU16" s="167" t="s">
+      <c r="BU16" s="185" t="s">
         <v>755</v>
       </c>
-      <c r="BV16" s="167" t="s">
+      <c r="BV16" s="185" t="s">
         <v>766</v>
       </c>
-      <c r="BW16" s="167" t="s">
+      <c r="BW16" s="185" t="s">
         <v>859</v>
       </c>
-      <c r="BX16" s="167" t="s">
+      <c r="BX16" s="185" t="s">
         <v>860</v>
       </c>
-      <c r="BY16" s="167" t="s">
+      <c r="BY16" s="185" t="s">
         <v>861</v>
       </c>
-      <c r="BZ16" s="167" t="s">
+      <c r="BZ16" s="185" t="s">
         <v>862</v>
       </c>
-      <c r="CA16" s="167" t="s">
+      <c r="CA16" s="185" t="s">
         <v>863</v>
       </c>
-      <c r="CB16" s="167" t="s">
+      <c r="CB16" s="185" t="s">
         <v>864</v>
       </c>
-      <c r="CC16" s="165" t="s">
+      <c r="CC16" s="183" t="s">
         <v>865</v>
       </c>
-      <c r="CD16" s="174" t="s">
+      <c r="CD16" s="214" t="s">
         <v>892</v>
       </c>
-      <c r="CE16" s="174" t="s">
+      <c r="CE16" s="214" t="s">
         <v>895</v>
       </c>
-      <c r="CF16" s="174" t="s">
+      <c r="CF16" s="214" t="s">
         <v>893</v>
       </c>
-      <c r="CG16" s="176" t="s">
+      <c r="CG16" s="269" t="s">
         <v>894</v>
       </c>
+      <c r="CH16" s="271" t="s">
+        <v>896</v>
+      </c>
     </row>
-    <row r="17" spans="1:85" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="227"/>
-      <c r="B17" s="229"/>
-      <c r="C17" s="229"/>
-      <c r="D17" s="229"/>
-      <c r="E17" s="229"/>
-      <c r="F17" s="229"/>
-      <c r="G17" s="229"/>
-      <c r="H17" s="229"/>
-      <c r="I17" s="241"/>
-      <c r="J17" s="229"/>
-      <c r="K17" s="235"/>
-      <c r="L17" s="237"/>
-      <c r="M17" s="215"/>
-      <c r="N17" s="215"/>
-      <c r="O17" s="239"/>
-      <c r="P17" s="231"/>
-      <c r="Q17" s="233"/>
-      <c r="R17" s="194"/>
-      <c r="S17" s="194"/>
-      <c r="T17" s="194"/>
-      <c r="U17" s="194"/>
-      <c r="V17" s="243"/>
-      <c r="W17" s="194"/>
-      <c r="X17" s="194"/>
-      <c r="Y17" s="194"/>
-      <c r="Z17" s="194"/>
-      <c r="AA17" s="194"/>
-      <c r="AB17" s="194"/>
-      <c r="AC17" s="194"/>
-      <c r="AD17" s="194"/>
-      <c r="AE17" s="194"/>
-      <c r="AF17" s="194"/>
-      <c r="AG17" s="194"/>
-      <c r="AH17" s="196"/>
-      <c r="AI17" s="198"/>
-      <c r="AJ17" s="245"/>
-      <c r="AK17" s="245"/>
-      <c r="AL17" s="247"/>
-      <c r="AM17" s="249"/>
-      <c r="AN17" s="208"/>
-      <c r="AO17" s="208"/>
-      <c r="AP17" s="174"/>
-      <c r="AQ17" s="211"/>
-      <c r="AR17" s="211"/>
-      <c r="AS17" s="213"/>
-      <c r="AT17" s="200"/>
-      <c r="AU17" s="202"/>
-      <c r="AV17" s="202"/>
-      <c r="AW17" s="206"/>
-      <c r="AX17" s="186"/>
-      <c r="AY17" s="186"/>
-      <c r="AZ17" s="188"/>
-      <c r="BA17" s="190"/>
-      <c r="BB17" s="192"/>
-      <c r="BC17" s="192"/>
-      <c r="BD17" s="215"/>
-      <c r="BE17" s="217"/>
-      <c r="BF17" s="217"/>
-      <c r="BG17" s="225"/>
-      <c r="BH17" s="184"/>
-      <c r="BI17" s="219"/>
-      <c r="BJ17" s="219"/>
-      <c r="BK17" s="221"/>
-      <c r="BL17" s="223"/>
-      <c r="BM17" s="223"/>
-      <c r="BN17" s="204"/>
-      <c r="BO17" s="178"/>
-      <c r="BP17" s="180"/>
-      <c r="BQ17" s="182"/>
-      <c r="BR17" s="182"/>
-      <c r="BS17" s="168"/>
-      <c r="BT17" s="180"/>
-      <c r="BU17" s="168"/>
-      <c r="BV17" s="168"/>
-      <c r="BW17" s="168"/>
-      <c r="BX17" s="168"/>
-      <c r="BY17" s="168"/>
-      <c r="BZ17" s="168"/>
-      <c r="CA17" s="168"/>
-      <c r="CB17" s="168"/>
-      <c r="CC17" s="166"/>
-      <c r="CD17" s="175"/>
-      <c r="CE17" s="175"/>
-      <c r="CF17" s="175"/>
-      <c r="CG17" s="158"/>
+    <row r="17" spans="1:86" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="224"/>
+      <c r="B17" s="226"/>
+      <c r="C17" s="226"/>
+      <c r="D17" s="226"/>
+      <c r="E17" s="226"/>
+      <c r="F17" s="226"/>
+      <c r="G17" s="226"/>
+      <c r="H17" s="226"/>
+      <c r="I17" s="228"/>
+      <c r="J17" s="226"/>
+      <c r="K17" s="230"/>
+      <c r="L17" s="232"/>
+      <c r="M17" s="176"/>
+      <c r="N17" s="176"/>
+      <c r="O17" s="234"/>
+      <c r="P17" s="236"/>
+      <c r="Q17" s="238"/>
+      <c r="R17" s="240"/>
+      <c r="S17" s="240"/>
+      <c r="T17" s="240"/>
+      <c r="U17" s="240"/>
+      <c r="V17" s="252"/>
+      <c r="W17" s="240"/>
+      <c r="X17" s="240"/>
+      <c r="Y17" s="240"/>
+      <c r="Z17" s="240"/>
+      <c r="AA17" s="240"/>
+      <c r="AB17" s="240"/>
+      <c r="AC17" s="240"/>
+      <c r="AD17" s="240"/>
+      <c r="AE17" s="240"/>
+      <c r="AF17" s="240"/>
+      <c r="AG17" s="240"/>
+      <c r="AH17" s="202"/>
+      <c r="AI17" s="204"/>
+      <c r="AJ17" s="206"/>
+      <c r="AK17" s="206"/>
+      <c r="AL17" s="208"/>
+      <c r="AM17" s="210"/>
+      <c r="AN17" s="212"/>
+      <c r="AO17" s="212"/>
+      <c r="AP17" s="214"/>
+      <c r="AQ17" s="180"/>
+      <c r="AR17" s="180"/>
+      <c r="AS17" s="182"/>
+      <c r="AT17" s="160"/>
+      <c r="AU17" s="162"/>
+      <c r="AV17" s="162"/>
+      <c r="AW17" s="164"/>
+      <c r="AX17" s="166"/>
+      <c r="AY17" s="166"/>
+      <c r="AZ17" s="168"/>
+      <c r="BA17" s="172"/>
+      <c r="BB17" s="178"/>
+      <c r="BC17" s="178"/>
+      <c r="BD17" s="176"/>
+      <c r="BE17" s="174"/>
+      <c r="BF17" s="174"/>
+      <c r="BG17" s="170"/>
+      <c r="BH17" s="256"/>
+      <c r="BI17" s="200"/>
+      <c r="BJ17" s="200"/>
+      <c r="BK17" s="198"/>
+      <c r="BL17" s="194"/>
+      <c r="BM17" s="194"/>
+      <c r="BN17" s="196"/>
+      <c r="BO17" s="192"/>
+      <c r="BP17" s="188"/>
+      <c r="BQ17" s="190"/>
+      <c r="BR17" s="190"/>
+      <c r="BS17" s="186"/>
+      <c r="BT17" s="188"/>
+      <c r="BU17" s="186"/>
+      <c r="BV17" s="186"/>
+      <c r="BW17" s="186"/>
+      <c r="BX17" s="186"/>
+      <c r="BY17" s="186"/>
+      <c r="BZ17" s="186"/>
+      <c r="CA17" s="186"/>
+      <c r="CB17" s="186"/>
+      <c r="CC17" s="184"/>
+      <c r="CD17" s="257"/>
+      <c r="CE17" s="257"/>
+      <c r="CF17" s="257"/>
+      <c r="CG17" s="259"/>
+      <c r="CH17" s="272"/>
     </row>
-    <row r="18" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -15862,8 +15903,9 @@
       <c r="CE18" s="155"/>
       <c r="CF18" s="155"/>
       <c r="CG18" s="156"/>
+      <c r="CH18" s="274"/>
     </row>
-    <row r="19" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -15953,8 +15995,9 @@
       <c r="CE19" s="155"/>
       <c r="CF19" s="155"/>
       <c r="CG19" s="156"/>
+      <c r="CH19" s="274"/>
     </row>
-    <row r="20" spans="1:85" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:86" ht="11" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
@@ -16042,24 +16085,259 @@
       <c r="CE20" s="74"/>
       <c r="CF20" s="74"/>
       <c r="CG20" s="153"/>
+      <c r="CH20" s="273"/>
     </row>
   </sheetData>
-  <mergeCells count="285">
-    <mergeCell ref="AT1:AZ2"/>
-    <mergeCell ref="AT3:AT4"/>
-    <mergeCell ref="AU3:AU4"/>
-    <mergeCell ref="AV3:AV4"/>
-    <mergeCell ref="AW3:AW4"/>
-    <mergeCell ref="AX3:AX4"/>
-    <mergeCell ref="AY3:AY4"/>
-    <mergeCell ref="AZ3:AZ4"/>
-    <mergeCell ref="BG3:BG4"/>
-    <mergeCell ref="BA3:BA4"/>
-    <mergeCell ref="BF3:BF4"/>
-    <mergeCell ref="BE3:BE4"/>
-    <mergeCell ref="BD3:BD4"/>
-    <mergeCell ref="BC3:BC4"/>
-    <mergeCell ref="BB3:BB4"/>
+  <mergeCells count="288">
+    <mergeCell ref="CH3:CH4"/>
+    <mergeCell ref="CH9:CH10"/>
+    <mergeCell ref="CH16:CH17"/>
+    <mergeCell ref="CG3:CG4"/>
+    <mergeCell ref="CD1:CG2"/>
+    <mergeCell ref="CC16:CC17"/>
+    <mergeCell ref="BX16:BX17"/>
+    <mergeCell ref="BY16:BY17"/>
+    <mergeCell ref="BZ16:BZ17"/>
+    <mergeCell ref="CA16:CA17"/>
+    <mergeCell ref="CB16:CB17"/>
+    <mergeCell ref="BZ9:BZ10"/>
+    <mergeCell ref="CA9:CA10"/>
+    <mergeCell ref="BO1:CC2"/>
+    <mergeCell ref="CD7:CG8"/>
+    <mergeCell ref="CD9:CD10"/>
+    <mergeCell ref="CE9:CE10"/>
+    <mergeCell ref="CF9:CF10"/>
+    <mergeCell ref="CG9:CG10"/>
+    <mergeCell ref="CD14:CG15"/>
+    <mergeCell ref="CD16:CD17"/>
+    <mergeCell ref="CE16:CE17"/>
+    <mergeCell ref="CF16:CF17"/>
+    <mergeCell ref="CG16:CG17"/>
+    <mergeCell ref="BV16:BV17"/>
+    <mergeCell ref="BW16:BW17"/>
+    <mergeCell ref="BO16:BO17"/>
+    <mergeCell ref="BP16:BP17"/>
+    <mergeCell ref="BQ16:BQ17"/>
+    <mergeCell ref="BR16:BR17"/>
+    <mergeCell ref="CD3:CD4"/>
+    <mergeCell ref="CE3:CE4"/>
+    <mergeCell ref="CF3:CF4"/>
+    <mergeCell ref="BH16:BH17"/>
+    <mergeCell ref="AY16:AY17"/>
+    <mergeCell ref="AZ16:AZ17"/>
+    <mergeCell ref="BA16:BA17"/>
+    <mergeCell ref="BB16:BB17"/>
+    <mergeCell ref="BC16:BC17"/>
+    <mergeCell ref="BS16:BS17"/>
+    <mergeCell ref="BT16:BT17"/>
+    <mergeCell ref="BU16:BU17"/>
+    <mergeCell ref="BN9:BN10"/>
+    <mergeCell ref="BO9:BO10"/>
+    <mergeCell ref="BR9:BR10"/>
+    <mergeCell ref="BS9:BS10"/>
+    <mergeCell ref="BH3:BH4"/>
+    <mergeCell ref="AF16:AF17"/>
+    <mergeCell ref="AG16:AG17"/>
+    <mergeCell ref="AH16:AH17"/>
+    <mergeCell ref="AI16:AI17"/>
+    <mergeCell ref="AT16:AT17"/>
+    <mergeCell ref="AU16:AU17"/>
+    <mergeCell ref="AV16:AV17"/>
+    <mergeCell ref="BN16:BN17"/>
+    <mergeCell ref="AW16:AW17"/>
+    <mergeCell ref="AX16:AX17"/>
+    <mergeCell ref="AO16:AO17"/>
+    <mergeCell ref="AP16:AP17"/>
+    <mergeCell ref="AQ16:AQ17"/>
+    <mergeCell ref="AR16:AR17"/>
+    <mergeCell ref="AS16:AS17"/>
+    <mergeCell ref="BD16:BD17"/>
+    <mergeCell ref="BE16:BE17"/>
+    <mergeCell ref="BI16:BI17"/>
+    <mergeCell ref="BJ16:BJ17"/>
+    <mergeCell ref="BK16:BK17"/>
+    <mergeCell ref="BL16:BL17"/>
+    <mergeCell ref="BM16:BM17"/>
+    <mergeCell ref="BF16:BF17"/>
+    <mergeCell ref="BG16:BG17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="S16:S17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="T16:T17"/>
+    <mergeCell ref="Z16:Z17"/>
+    <mergeCell ref="AA16:AA17"/>
+    <mergeCell ref="AB16:AB17"/>
+    <mergeCell ref="AC16:AC17"/>
+    <mergeCell ref="AD16:AD17"/>
+    <mergeCell ref="U16:U17"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="X16:X17"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="AJ16:AJ17"/>
+    <mergeCell ref="AK16:AK17"/>
+    <mergeCell ref="AL16:AL17"/>
+    <mergeCell ref="AM16:AM17"/>
+    <mergeCell ref="AN16:AN17"/>
+    <mergeCell ref="AE16:AE17"/>
+    <mergeCell ref="CB9:CB10"/>
+    <mergeCell ref="CC9:CC10"/>
+    <mergeCell ref="A14:K15"/>
+    <mergeCell ref="L14:P15"/>
+    <mergeCell ref="Q14:AH15"/>
+    <mergeCell ref="AI14:AL15"/>
+    <mergeCell ref="AM14:AS15"/>
+    <mergeCell ref="AT14:AZ15"/>
+    <mergeCell ref="BA14:BG15"/>
+    <mergeCell ref="BH14:BN15"/>
+    <mergeCell ref="BO14:CC15"/>
+    <mergeCell ref="BU9:BU10"/>
+    <mergeCell ref="BV9:BV10"/>
+    <mergeCell ref="BW9:BW10"/>
+    <mergeCell ref="BX9:BX10"/>
+    <mergeCell ref="BY9:BY10"/>
+    <mergeCell ref="BP9:BP10"/>
+    <mergeCell ref="BQ9:BQ10"/>
+    <mergeCell ref="BT9:BT10"/>
+    <mergeCell ref="BK9:BK10"/>
+    <mergeCell ref="AX9:AX10"/>
+    <mergeCell ref="AY9:AY10"/>
+    <mergeCell ref="AZ9:AZ10"/>
+    <mergeCell ref="BL9:BL10"/>
+    <mergeCell ref="BM9:BM10"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BH9:BH10"/>
+    <mergeCell ref="BI9:BI10"/>
+    <mergeCell ref="BJ9:BJ10"/>
+    <mergeCell ref="BD9:BD10"/>
+    <mergeCell ref="BE9:BE10"/>
+    <mergeCell ref="AU9:AU10"/>
+    <mergeCell ref="AL9:AL10"/>
+    <mergeCell ref="AM9:AM10"/>
+    <mergeCell ref="AN9:AN10"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="BA9:BA10"/>
+    <mergeCell ref="BB9:BB10"/>
+    <mergeCell ref="BC9:BC10"/>
+    <mergeCell ref="AV9:AV10"/>
+    <mergeCell ref="AW9:AW10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="AS9:AS10"/>
+    <mergeCell ref="AT9:AT10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="AT7:AZ8"/>
+    <mergeCell ref="BA7:BG8"/>
+    <mergeCell ref="BH7:BN8"/>
+    <mergeCell ref="BO7:CC8"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="AG9:AG10"/>
+    <mergeCell ref="AH9:AH10"/>
+    <mergeCell ref="AI9:AI10"/>
+    <mergeCell ref="AJ9:AJ10"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="A7:K8"/>
+    <mergeCell ref="L7:P8"/>
+    <mergeCell ref="Q7:AH8"/>
+    <mergeCell ref="AI7:AL8"/>
+    <mergeCell ref="AM7:AS8"/>
+    <mergeCell ref="Q1:AH2"/>
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="L1:P2"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="AI1:AL2"/>
+    <mergeCell ref="AM1:AS2"/>
+    <mergeCell ref="BA1:BG2"/>
+    <mergeCell ref="BH1:BN2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="AG3:AG4"/>
+    <mergeCell ref="AH3:AH4"/>
+    <mergeCell ref="AI3:AI4"/>
+    <mergeCell ref="AJ3:AJ4"/>
+    <mergeCell ref="AK3:AK4"/>
+    <mergeCell ref="AL3:AL4"/>
+    <mergeCell ref="AM3:AM4"/>
+    <mergeCell ref="AN3:AN4"/>
+    <mergeCell ref="AO3:AO4"/>
+    <mergeCell ref="AP3:AP4"/>
     <mergeCell ref="AQ3:AQ4"/>
     <mergeCell ref="AR3:AR4"/>
     <mergeCell ref="AS3:AS4"/>
@@ -16084,252 +16362,21 @@
     <mergeCell ref="BK3:BK4"/>
     <mergeCell ref="BJ3:BJ4"/>
     <mergeCell ref="BI3:BI4"/>
-    <mergeCell ref="AH3:AH4"/>
-    <mergeCell ref="AI3:AI4"/>
-    <mergeCell ref="AJ3:AJ4"/>
-    <mergeCell ref="AK3:AK4"/>
-    <mergeCell ref="AL3:AL4"/>
-    <mergeCell ref="AM3:AM4"/>
-    <mergeCell ref="AN3:AN4"/>
-    <mergeCell ref="AO3:AO4"/>
-    <mergeCell ref="AP3:AP4"/>
-    <mergeCell ref="AI1:AL2"/>
-    <mergeCell ref="AM1:AS2"/>
-    <mergeCell ref="BA1:BG2"/>
-    <mergeCell ref="BH1:BN2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="AG3:AG4"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="A7:K8"/>
-    <mergeCell ref="L7:P8"/>
-    <mergeCell ref="Q7:AH8"/>
-    <mergeCell ref="AI7:AL8"/>
-    <mergeCell ref="AM7:AS8"/>
-    <mergeCell ref="Q1:AH2"/>
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="L1:P2"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="AT7:AZ8"/>
-    <mergeCell ref="BA7:BG8"/>
-    <mergeCell ref="BH7:BN8"/>
-    <mergeCell ref="BO7:CC8"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="AG9:AG10"/>
-    <mergeCell ref="AH9:AH10"/>
-    <mergeCell ref="AI9:AI10"/>
-    <mergeCell ref="AJ9:AJ10"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="AS9:AS10"/>
-    <mergeCell ref="AT9:AT10"/>
-    <mergeCell ref="AU9:AU10"/>
-    <mergeCell ref="AL9:AL10"/>
-    <mergeCell ref="AM9:AM10"/>
-    <mergeCell ref="AN9:AN10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="BA9:BA10"/>
-    <mergeCell ref="BB9:BB10"/>
-    <mergeCell ref="BC9:BC10"/>
-    <mergeCell ref="AV9:AV10"/>
-    <mergeCell ref="AW9:AW10"/>
-    <mergeCell ref="BT9:BT10"/>
-    <mergeCell ref="BK9:BK10"/>
-    <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="AY9:AY10"/>
-    <mergeCell ref="AZ9:AZ10"/>
-    <mergeCell ref="BL9:BL10"/>
-    <mergeCell ref="BM9:BM10"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BH9:BH10"/>
-    <mergeCell ref="BI9:BI10"/>
-    <mergeCell ref="BJ9:BJ10"/>
-    <mergeCell ref="BD9:BD10"/>
-    <mergeCell ref="BE9:BE10"/>
-    <mergeCell ref="AJ16:AJ17"/>
-    <mergeCell ref="AK16:AK17"/>
-    <mergeCell ref="AL16:AL17"/>
-    <mergeCell ref="AM16:AM17"/>
-    <mergeCell ref="AN16:AN17"/>
-    <mergeCell ref="AE16:AE17"/>
-    <mergeCell ref="CB9:CB10"/>
-    <mergeCell ref="CC9:CC10"/>
-    <mergeCell ref="A14:K15"/>
-    <mergeCell ref="L14:P15"/>
-    <mergeCell ref="Q14:AH15"/>
-    <mergeCell ref="AI14:AL15"/>
-    <mergeCell ref="AM14:AS15"/>
-    <mergeCell ref="AT14:AZ15"/>
-    <mergeCell ref="BA14:BG15"/>
-    <mergeCell ref="BH14:BN15"/>
-    <mergeCell ref="BO14:CC15"/>
-    <mergeCell ref="BU9:BU10"/>
-    <mergeCell ref="BV9:BV10"/>
-    <mergeCell ref="BW9:BW10"/>
-    <mergeCell ref="BX9:BX10"/>
-    <mergeCell ref="BY9:BY10"/>
-    <mergeCell ref="BP9:BP10"/>
-    <mergeCell ref="BQ9:BQ10"/>
-    <mergeCell ref="T16:T17"/>
-    <mergeCell ref="Z16:Z17"/>
-    <mergeCell ref="AA16:AA17"/>
-    <mergeCell ref="AB16:AB17"/>
-    <mergeCell ref="AC16:AC17"/>
-    <mergeCell ref="AD16:AD17"/>
-    <mergeCell ref="U16:U17"/>
-    <mergeCell ref="V16:V17"/>
-    <mergeCell ref="W16:W17"/>
-    <mergeCell ref="X16:X17"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="P16:P17"/>
-    <mergeCell ref="Q16:Q17"/>
-    <mergeCell ref="R16:R17"/>
-    <mergeCell ref="S16:S17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="AF16:AF17"/>
-    <mergeCell ref="AG16:AG17"/>
-    <mergeCell ref="AH16:AH17"/>
-    <mergeCell ref="AI16:AI17"/>
-    <mergeCell ref="AT16:AT17"/>
-    <mergeCell ref="AU16:AU17"/>
-    <mergeCell ref="AV16:AV17"/>
-    <mergeCell ref="BN16:BN17"/>
-    <mergeCell ref="AW16:AW17"/>
-    <mergeCell ref="AX16:AX17"/>
-    <mergeCell ref="AO16:AO17"/>
-    <mergeCell ref="AP16:AP17"/>
-    <mergeCell ref="AQ16:AQ17"/>
-    <mergeCell ref="AR16:AR17"/>
-    <mergeCell ref="AS16:AS17"/>
-    <mergeCell ref="BD16:BD17"/>
-    <mergeCell ref="BE16:BE17"/>
-    <mergeCell ref="BI16:BI17"/>
-    <mergeCell ref="BJ16:BJ17"/>
-    <mergeCell ref="BK16:BK17"/>
-    <mergeCell ref="BL16:BL17"/>
-    <mergeCell ref="BM16:BM17"/>
-    <mergeCell ref="BF16:BF17"/>
-    <mergeCell ref="BG16:BG17"/>
-    <mergeCell ref="BP16:BP17"/>
-    <mergeCell ref="BQ16:BQ17"/>
-    <mergeCell ref="BR16:BR17"/>
-    <mergeCell ref="CD3:CD4"/>
-    <mergeCell ref="CE3:CE4"/>
-    <mergeCell ref="CF3:CF4"/>
-    <mergeCell ref="BH16:BH17"/>
-    <mergeCell ref="AY16:AY17"/>
-    <mergeCell ref="AZ16:AZ17"/>
-    <mergeCell ref="BA16:BA17"/>
-    <mergeCell ref="BB16:BB17"/>
-    <mergeCell ref="BC16:BC17"/>
-    <mergeCell ref="BS16:BS17"/>
-    <mergeCell ref="BT16:BT17"/>
-    <mergeCell ref="BU16:BU17"/>
-    <mergeCell ref="BN9:BN10"/>
-    <mergeCell ref="BO9:BO10"/>
-    <mergeCell ref="BR9:BR10"/>
-    <mergeCell ref="BS9:BS10"/>
-    <mergeCell ref="BH3:BH4"/>
-    <mergeCell ref="CG3:CG4"/>
-    <mergeCell ref="CD1:CG2"/>
-    <mergeCell ref="CC16:CC17"/>
-    <mergeCell ref="BX16:BX17"/>
-    <mergeCell ref="BY16:BY17"/>
-    <mergeCell ref="BZ16:BZ17"/>
-    <mergeCell ref="CA16:CA17"/>
-    <mergeCell ref="CB16:CB17"/>
-    <mergeCell ref="BZ9:BZ10"/>
-    <mergeCell ref="CA9:CA10"/>
-    <mergeCell ref="BO1:CC2"/>
-    <mergeCell ref="CD7:CG8"/>
-    <mergeCell ref="CD9:CD10"/>
-    <mergeCell ref="CE9:CE10"/>
-    <mergeCell ref="CF9:CF10"/>
-    <mergeCell ref="CG9:CG10"/>
-    <mergeCell ref="CD14:CG15"/>
-    <mergeCell ref="CD16:CD17"/>
-    <mergeCell ref="CE16:CE17"/>
-    <mergeCell ref="CF16:CF17"/>
-    <mergeCell ref="CG16:CG17"/>
-    <mergeCell ref="BV16:BV17"/>
-    <mergeCell ref="BW16:BW17"/>
-    <mergeCell ref="BO16:BO17"/>
+    <mergeCell ref="AT1:AZ2"/>
+    <mergeCell ref="AT3:AT4"/>
+    <mergeCell ref="AU3:AU4"/>
+    <mergeCell ref="AV3:AV4"/>
+    <mergeCell ref="AW3:AW4"/>
+    <mergeCell ref="AX3:AX4"/>
+    <mergeCell ref="AY3:AY4"/>
+    <mergeCell ref="AZ3:AZ4"/>
+    <mergeCell ref="BG3:BG4"/>
+    <mergeCell ref="BA3:BA4"/>
+    <mergeCell ref="BF3:BF4"/>
+    <mergeCell ref="BE3:BE4"/>
+    <mergeCell ref="BD3:BD4"/>
+    <mergeCell ref="BC3:BC4"/>
+    <mergeCell ref="BB3:BB4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>